<commit_message>
get rid of "latest" mechanism in cache and add LRU cache to web service
</commit_message>
<xml_diff>
--- a/test/resources/unittest_DAZHO.xlsx
+++ b/test/resources/unittest_DAZHO.xlsx
@@ -768,7 +768,7 @@
     <row r="2" ht="18" customHeight="1">
       <c r="A2" s="24" t="inlineStr">
         <is>
-          <t>State Archives of Zhytomyr Region. The pre -Soviet period</t>
+          <t>Державний архів Житомирської області. Дорадянський період</t>
         </is>
       </c>
       <c r="B2" s="23" t="n"/>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B7" s="6" t="inlineStr">
         <is>
-          <t>Volyn Spiritual Consistory of Zhytomyr, Volyn Province</t>
+          <t>Волинська духовна консисторія м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C7" s="27" t="inlineStr">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="B8" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr County Court of Zhytomyr, Volyn Province</t>
+          <t>Житомирський повітовий суд м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C8" s="27" t="inlineStr">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B9" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Horoda Magistrate in Zhytomyr, Volyn Province</t>
+          <t>Житомирський городовий магістрат м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C9" s="27" t="inlineStr">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="B10" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr noble care of Zhytomyr, Volyn province</t>
+          <t>Житомирська дворянська опіка м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C10" s="27" t="inlineStr">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="B11" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volyn Horoda Magistrate of Nov.-Volynsky, Volyn province</t>
+          <t>Новоград-Волинський городовий магістрат м. Нов.-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C11" s="27" t="inlineStr">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volynsky County Court of Nov.-Volynsky, Volyn Province</t>
+          <t>Новоград-Волинський повітовий суд м. Нов.-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C12" s="27" t="inlineStr">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="B13" s="6" t="inlineStr">
         <is>
-          <t>Ovruch County Court of Ovruch, Volyn Province</t>
+          <t>Овруцький повітовий суд м. Овруч, Волинської губернії</t>
         </is>
       </c>
       <c r="C13" s="27" t="inlineStr">
@@ -1336,7 +1336,7 @@
       </c>
       <c r="B14" s="6" t="inlineStr">
         <is>
-          <t>Ovruch city magistrate in Ovruch, Volyn province</t>
+          <t>Овруцький городовий магістрат м. Овруч, Волинської губернії</t>
         </is>
       </c>
       <c r="C14" s="27" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B15" s="6" t="inlineStr">
         <is>
-          <t>Volyn Chief Court of Zhytomyr, Volyn Province</t>
+          <t>Волинський головний суд м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C15" s="27" t="inlineStr">
@@ -1426,7 +1426,7 @@
       </c>
       <c r="B16" s="6" t="inlineStr">
         <is>
-          <t>Volyn Chamber of Civil Court of Zhytomyr, Volyn Province</t>
+          <t>Волинська палата цивільного суду м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C16" s="27" t="inlineStr">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="B17" s="6" t="inlineStr">
         <is>
-          <t>Volyn Chamber of Criminal Court of Zhytomyr, Volyn Province</t>
+          <t>Волинська палата кримінального суду м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C17" s="27" t="inlineStr">
@@ -1516,7 +1516,7 @@
       </c>
       <c r="B18" s="6" t="inlineStr">
         <is>
-          <t>Volyn United Criminal and Civil Court of Zhytomyr, Volyn Province</t>
+          <t>Волинська об’єднана палата кримінального і цивільного суду м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C18" s="27" t="inlineStr">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="B19" s="6" t="inlineStr">
         <is>
-          <t>Volyn Conscious Court of Zhytomyr, Volyn Province</t>
+          <t>Волинський совісний суд м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C19" s="27" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="B20" s="6" t="inlineStr">
         <is>
-          <t>Volyn Liquidation Commission on Cancellation</t>
+          <t>Волинська ліквідаційна комісія по скасуванню боргів конфіскованих маєтків м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C20" s="27" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="B21" s="6" t="inlineStr">
         <is>
-          <t>Volyn Nadvirny Court of Zhytomyr, Volyn Province</t>
+          <t>Волинський надвірний суд м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C21" s="27" t="inlineStr">
@@ -1696,7 +1696,7 @@
       </c>
       <c r="B22" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr District Court of Zhytomyr, Volyn Province</t>
+          <t>Житомирський окружний суд м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C22" s="27" t="inlineStr">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="B23" s="6" t="inlineStr">
         <is>
-          <t>Senior notary of the Zhytomyr District Court of Zhytomyr, Volyn Province</t>
+          <t>Старший нотаріус Житомирського окружного суду м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C23" s="27" t="inlineStr">
@@ -1786,7 +1786,7 @@
       </c>
       <c r="B24" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr notary Przemensky Erazm Stepanovich Zhytomyr, Volyn Province</t>
+          <t>Житомирський нотаріус Пршеменський Єразм Степанович м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C24" s="27" t="inlineStr">
@@ -1831,7 +1831,7 @@
       </c>
       <c r="B25" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr notary Philippov Ivan Nikolaevich Zhytomyr, Volyn Province</t>
+          <t>Житомирський нотаріус Філіппов Іван Миколайович м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C25" s="27" t="inlineStr">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="B26" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr notary Kriger Petro Ivanovich Zhytomyr, Volyn Province</t>
+          <t>Житомирський нотаріус Крігер Петро Іванович м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C26" s="27" t="inlineStr">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="B27" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr notary Zavalievsky Andrey Vasilyevich Zhytomyr, Volyn Province</t>
+          <t>Житомирський нотаріус Завалієвський Андрій Васильович м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C27" s="27" t="inlineStr">
@@ -1966,7 +1966,7 @@
       </c>
       <c r="B28" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr notary Semkovsky Alexander Antonovich Zhytomyr, Volyn Province</t>
+          <t>Житомирський нотаріус Семковський Олександр Антонович м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C28" s="27" t="inlineStr">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="B29" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr notary Malevich Alexander Mikhailovich Zhytomyr, Volyn province</t>
+          <t>Житомирський нотаріус Малевич Олександр Михайлович м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C29" s="27" t="inlineStr">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="B30" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr notary Gromachevsky Semen Grigorovich, Zhytomyr, Volyn Province</t>
+          <t>Житомирський нотаріус Громачевський Семен Григорович м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C30" s="27" t="inlineStr">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="B31" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr notary Kotelevsky Ivan Mikhailovich Zhytomyr of Volyn Province</t>
+          <t>Житомирський нотаріус Котелевський Іван Михайлович м. Житомир Волинської губернії</t>
         </is>
       </c>
       <c r="C31" s="27" t="inlineStr">
@@ -2092,7 +2092,7 @@
       </c>
       <c r="B32" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr notary Kruger Augustus Fedorovich, Zhytomyr of Volyn Province</t>
+          <t>Житомирський нотаріус Крюгер Август Федорович м. Житомир Волинської губернії</t>
         </is>
       </c>
       <c r="C32" s="27" t="inlineStr">
@@ -2119,7 +2119,7 @@
       </c>
       <c r="B33" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr notary Radakov Petro Nikolaevich Zhytomyr of Volyn Province</t>
+          <t>Житомирський нотаріус Радаков Петро Миколайович м. Житомир Волинської губернії</t>
         </is>
       </c>
       <c r="C33" s="27" t="inlineStr">
@@ -2146,7 +2146,7 @@
       </c>
       <c r="B34" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr notary Zaitsev Mikhail Gerasimovich Zhytomyr, Volyn province</t>
+          <t>Житомирський нотаріус Зайцев Михайло Герасимович м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C34" s="27" t="inlineStr">
@@ -2173,7 +2173,7 @@
       </c>
       <c r="B35" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr notary Ivanov Alexander Mikhailovich Zhytomyr, Volyn province</t>
+          <t>Житомирський нотаріус Іванов Олександр Михайлович м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C35" s="27" t="inlineStr">
@@ -2200,7 +2200,7 @@
       </c>
       <c r="B36" s="6" t="inlineStr">
         <is>
-          <t>Chudniv notary Masyukevich Mykola Onufrievich M. Chudnov, Zhytomyr County</t>
+          <t>Чуднівський нотаріус Масюкевич Микола Онуфрійович м-ко Чуднів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C36" s="27" t="inlineStr">
@@ -2227,7 +2227,7 @@
       </c>
       <c r="B37" s="6" t="inlineStr">
         <is>
-          <t>Ovruch notary Olshansky Joseph Feofilovich Ovruch, Volyn Province</t>
+          <t>Овруцький нотаріус Ольшанський Йосип Феофілович м. Овруч, Волинської губернії</t>
         </is>
       </c>
       <c r="C37" s="27" t="inlineStr">
@@ -2254,7 +2254,7 @@
       </c>
       <c r="B38" s="6" t="inlineStr">
         <is>
-          <t>Ovruch notary Kukharenko Alexander Ivanovich Ovruch, Volyn Province</t>
+          <t>Овруцький нотаріус Кухаренко Олександр Іванович м. Овруч, Волинської губернії</t>
         </is>
       </c>
       <c r="C38" s="27" t="inlineStr">
@@ -2281,7 +2281,7 @@
       </c>
       <c r="B39" s="6" t="inlineStr">
         <is>
-          <t>Iscorostensky notary Kashin Ivan Ivanovich M-ko of Iscorosten, Ovruch County</t>
+          <t>Іскоростенський нотаріус Кашин Іван Іванович м-ко Іскоростень, Овруцького повіту</t>
         </is>
       </c>
       <c r="C39" s="27" t="inlineStr">
@@ -2308,7 +2308,7 @@
       </c>
       <c r="B40" s="6" t="inlineStr">
         <is>
-          <t>Nov.-Volynsky notary Lobko-Lobanovsky Yakov Nikolaevich Nov.-Volynsky, Volyn province</t>
+          <t>Нов.-Волинський нотаріус Лобко-Лобановський Яків Миколайович м. Нов.-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C40" s="27" t="inlineStr">
@@ -2335,7 +2335,7 @@
       </c>
       <c r="B41" s="6" t="inlineStr">
         <is>
-          <t>Nov.-Volynsky notary de-Lamer Karl Matviyevich Nov.-Volynsky, Volyn province</t>
+          <t>Нов.-Волинський нотаріус де-Лямер Карл Матвійович м. Нов.-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C41" s="27" t="inlineStr">
@@ -2362,7 +2362,7 @@
       </c>
       <c r="B42" s="6" t="inlineStr">
         <is>
-          <t>Nov.-Volynsky notary Senitsky Yevgeny Yevgenyevich Nov.-Volynskyi, Volyn Province</t>
+          <t>Нов.-Волинський нотаріус Сеницький Євген Євгенійович м. Нов.-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C42" s="27" t="inlineStr">
@@ -2389,7 +2389,7 @@
       </c>
       <c r="B43" s="6" t="inlineStr">
         <is>
-          <t>Nov.-Volyn notary Kashurnikov Afanasiy Semenovich Nov.-Volynskyi, Volyn province</t>
+          <t>Нов.-Волинський нотаріус Кашурніков Афанасій Семенович м. Нов.-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C43" s="27" t="inlineStr">
@@ -2416,7 +2416,7 @@
       </c>
       <c r="B44" s="6" t="inlineStr">
         <is>
-          <t>Lyubarsky notaryis Piasetsky Mykola Petrovich M-KO Lyubar, Nov.-Volyn County</t>
+          <t>Любарський нотаріс Пясецький Микола Петрович м-ко Любар, Нов.-Волинського повіту</t>
         </is>
       </c>
       <c r="C44" s="27" t="inlineStr">
@@ -2443,7 +2443,7 @@
       </c>
       <c r="B45" s="6" t="inlineStr">
         <is>
-          <t>Notary Grisinsky Oleksandr Alexandrovich M-ko Lubar, Nov.-Volyn County</t>
+          <t>Нотаріус Грудзинський Олександр Олександрович м-ко Любар, Нов.-Волинського повіту</t>
         </is>
       </c>
       <c r="C45" s="27" t="inlineStr">
@@ -2470,7 +2470,7 @@
       </c>
       <c r="B46" s="6" t="inlineStr">
         <is>
-          <t>Lyubarsky notary Zozulevich Mykola Semenovich M-ko Lubar, Nov.-Volyn County</t>
+          <t>Любарський нотаріус Зозулевич Микола Семенович м-ко Любар, Нов.-Волинського повіту</t>
         </is>
       </c>
       <c r="C46" s="27" t="inlineStr">
@@ -2497,7 +2497,7 @@
       </c>
       <c r="B47" s="6" t="inlineStr">
         <is>
-          <t>Volyn Chamber of State Property of Zhytomyr, Volyn Province</t>
+          <t>Волинська палата державного майна м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C47" s="27" t="inlineStr">
@@ -2524,7 +2524,7 @@
       </c>
       <c r="B48" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Drawing Crawl of Zhytomyr, Volyn Province</t>
+          <t>Волинська губернська креслярня м. Житомир,Волинської губернії</t>
         </is>
       </c>
       <c r="C48" s="27" t="inlineStr">
@@ -2551,7 +2551,7 @@
       </c>
       <c r="B49" s="6" t="inlineStr">
         <is>
-          <t>Nov.-Volyn County Land Management Commission of Nov.-Volynsky, Volyn Province</t>
+          <t>Нов.-Волинська повітова землевпорядна комісія м. Нов.-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C49" s="27" t="inlineStr">
@@ -2578,7 +2578,7 @@
       </c>
       <c r="B50" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr City Administration of Zhytomyr, Volyn Province</t>
+          <t>Житомирська міська управа м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C50" s="27" t="inlineStr">
@@ -2605,7 +2605,7 @@
       </c>
       <c r="B51" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr City Police Department of Zhytomyr, Volyn Province</t>
+          <t>Житомирське міське поліцейське управління м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C51" s="27" t="inlineStr">
@@ -2632,7 +2632,7 @@
       </c>
       <c r="B52" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr City Duma</t>
+          <t>Житомирська міська дума</t>
         </is>
       </c>
       <c r="C52" s="27" t="inlineStr">
@@ -2659,7 +2659,7 @@
       </c>
       <c r="B53" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Handicraft Directorate of Zhytomyr, Volyn Province</t>
+          <t>Житомирська реміснича управа м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C53" s="27" t="inlineStr">
@@ -2686,7 +2686,7 @@
       </c>
       <c r="B54" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr bourgeois office of Zhytomyr, Volyn province</t>
+          <t>Житомирська міщанська управа м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C54" s="27" t="inlineStr">
@@ -2713,7 +2713,7 @@
       </c>
       <c r="B55" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Board of Zhytomyr, Volyn Province</t>
+          <t>Волинське губернське правління м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C55" s="27" t="inlineStr">
@@ -2740,7 +2740,7 @@
       </c>
       <c r="B56" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr County Land Management Commission of Zhytomyr, Volyn Province</t>
+          <t>Житомирська повітова землевпорядкована комісія м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C56" s="27" t="inlineStr">
@@ -2767,7 +2767,7 @@
       </c>
       <c r="B57" s="6" t="inlineStr">
         <is>
-          <t>The office of Volyn governor of Zhytomyr, Volyn province</t>
+          <t>Канцелярія Волинського губернатора м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C57" s="27" t="inlineStr">
@@ -2794,7 +2794,7 @@
       </c>
       <c r="B58" s="6" t="inlineStr">
         <is>
-          <t>Directorate of People's Schools of Volyn Province, Zhytomyr, Volyn Province</t>
+          <t>Дирекція народних училищ Волинської губернії, м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C58" s="27" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="B59" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr 1st Men's Gymnasium</t>
+          <t>Житомирська 1-ша чоловіча гімназія</t>
         </is>
       </c>
       <c r="C59" s="27" t="inlineStr">
@@ -2848,7 +2848,7 @@
       </c>
       <c r="B60" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr 2nd Men's Gymnasium of Zhytomyr, Volyn Province</t>
+          <t>Житомирська 2-га чоловіча гімназія м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C60" s="27" t="inlineStr">
@@ -2875,7 +2875,7 @@
       </c>
       <c r="B61" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Mariinsky Women's Gymnasium of Zhytomyr. Volyn province</t>
+          <t>Житомирська Маріїнська жіноча гімназія м. Житомир. Волинської губернії</t>
         </is>
       </c>
       <c r="C61" s="27" t="inlineStr">
@@ -2902,7 +2902,7 @@
       </c>
       <c r="B62" s="6" t="inlineStr">
         <is>
-          <t>Teacher Seminary of the Southwestern Territory. Korostyshiv Teachers' Seminary of Korostyshiv, Radomysl County</t>
+          <t>Учительська семінарія Південно-Західного краю. Коростишівська учительська семінарія м-ко Коростишів, Радомисльського повіту</t>
         </is>
       </c>
       <c r="C62" s="27" t="inlineStr">
@@ -2929,7 +2929,7 @@
       </c>
       <c r="B63" s="6" t="inlineStr">
         <is>
-          <t>Volyn Control Chamber of Zhytomyr, Volyn Province</t>
+          <t>Волинська контрольна палата м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C63" s="27" t="inlineStr">
@@ -2956,7 +2956,7 @@
       </c>
       <c r="B64" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial for Elections to the State Duma of the 1st convocation Commission of Zhytomyr</t>
+          <t>Волинська губернська у справах про вибори до Державної Думи 1-го скликання комісія м. Житомир</t>
         </is>
       </c>
       <c r="C64" s="27" t="inlineStr">
@@ -2983,7 +2983,7 @@
       </c>
       <c r="B65" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Women's Gymnasium of St. Anastasia Zhytomyr, Volyn Province</t>
+          <t>Житомирська жіноча гімназія святої Анастасії м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C65" s="27" t="inlineStr">
@@ -3010,7 +3010,7 @@
       </c>
       <c r="B66" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr private eight -class male and women's commercial school NA Rezova Zhytomyr, Volyn province</t>
+          <t>Житомирське приватне восьмикласне чоловіче і жіноче комерційне училище Н. А. Ремезової м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C66" s="27" t="inlineStr">
@@ -3037,7 +3037,7 @@
       </c>
       <c r="B67" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr City Credit Society of Zhytomyr, Volyn Province</t>
+          <t>Житомирське міське кредитне товариство м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C67" s="27" t="inlineStr">
@@ -3064,7 +3064,7 @@
       </c>
       <c r="B68" s="6" t="inlineStr">
         <is>
-          <t>Volyn Zemsky School of Feldsers Zhytomyr, Volyn Province</t>
+          <t>Волинська земська школа фельдшерів м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C68" s="27" t="inlineStr">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="B69" s="6" t="inlineStr">
         <is>
-          <t>Visitor of Roman Catholic monasteries of Lutsk-Zhytomyr Diocese of Zhytomyr, Volyn Province</t>
+          <t>Візитатор римо-католицьких монастирів Луцько-Житомирської єпархії м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C69" s="27" t="inlineStr">
@@ -3118,7 +3118,7 @@
       </c>
       <c r="B70" s="6" t="inlineStr">
         <is>
-          <t>Lyubar Monastery</t>
+          <t>Любарський жіночий монастир м-ко Любар, Нов.-Волинського повіту</t>
         </is>
       </c>
       <c r="C70" s="27" t="inlineStr">
@@ -3145,7 +3145,7 @@
       </c>
       <c r="B71" s="6" t="inlineStr">
         <is>
-          <t>Triirsky two -class male Transfiguration Monastery Trigoria, Troyanivska parish, Zhytomyr county</t>
+          <t>Тригірський двокласний чоловічий Преображенський монастир с. Тригір'я, Троянівської волості, Житомирського повіту</t>
         </is>
       </c>
       <c r="C71" s="27" t="inlineStr">
@@ -3172,7 +3172,7 @@
       </c>
       <c r="B72" s="6" t="inlineStr">
         <is>
-          <t>Lubarsky Basilian Monastery</t>
+          <t>Любарський Базиліанський чоловічий монастир м-ко Любар, Нов.-Волинського повіту</t>
         </is>
       </c>
       <c r="C72" s="27" t="inlineStr">
@@ -3199,7 +3199,7 @@
       </c>
       <c r="B73" s="6" t="inlineStr">
         <is>
-          <t>Lubarsky Right-class St. George's Men's Monastery of Mr. Lubar. Nov.-Volyn county</t>
+          <t>Любарський правосласний Георгіївський чоловічий двокласний монастир м-ко Любар. Нов.-Волинського повіту</t>
         </is>
       </c>
       <c r="C73" s="27" t="inlineStr">
@@ -3226,7 +3226,7 @@
       </c>
       <c r="B74" s="6" t="inlineStr">
         <is>
-          <t>Lutsk-Zhytomyr Roman Catholic Cathedral Capital of Zhytomyr, Volyn Province</t>
+          <t>Луцько-Житомирський римо-католицький кафедральний капітул м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C74" s="27" t="inlineStr">
@@ -3253,7 +3253,7 @@
       </c>
       <c r="B75" s="6" t="inlineStr">
         <is>
-          <t>Volyn Local Administration of the Russian Society of the Red Cross of Zhytomyr, Volyn Province</t>
+          <t>Волинське місцеве управління Російського товариства Червоного Хреста м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C75" s="27" t="inlineStr">
@@ -3280,7 +3280,7 @@
       </c>
       <c r="B76" s="6" t="inlineStr">
         <is>
-          <t>The 6th state of Zhytomyr district, Zhytomyr, Volyn province</t>
+          <t>Пристав 6-го стану Житомирського повіту, м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C76" s="27" t="inlineStr">
@@ -3307,7 +3307,7 @@
       </c>
       <c r="B77" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volyn State Savings Cashier No. 254 Nov.-Volynsky, Volyn Province</t>
+          <t>Новоград-Волинська державна ощадна каса № 254 м. Нов.-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C77" s="27" t="inlineStr">
@@ -3334,7 +3334,7 @@
       </c>
       <c r="B78" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volyn County Treasury, Nov.-Vol., Volyn Province</t>
+          <t>Новоград-Волинське повітове казначейство м. Нов.-Вол., Волинської губернії</t>
         </is>
       </c>
       <c r="C78" s="27" t="inlineStr">
@@ -3361,7 +3361,7 @@
       </c>
       <c r="B79" s="6" t="inlineStr">
         <is>
-          <t>The Board of the Zhytomyr City Society Mutual from the Fire of Property Insurance of Zhytomyr, Volyn Province</t>
+          <t>Правління Житомирського міського товариства взаємного від вогню страхування майна м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C79" s="27" t="inlineStr">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="B80" s="6" t="inlineStr">
         <is>
-          <t>The Holm-Volyn Department of Agriculture and State Property of Zhytomyr. Volyn province</t>
+          <t>Холмсько-Волинське управління землеробства і державного майна м. Житомир. Волинської губернії</t>
         </is>
       </c>
       <c r="C80" s="27" t="inlineStr">
@@ -3415,7 +3415,7 @@
       </c>
       <c r="B81" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Forest Protection Committee of Zhytomyr, Volyn Province</t>
+          <t>Волинський губернський лісоохоронний комітет м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C81" s="27" t="inlineStr">
@@ -3442,7 +3442,7 @@
       </c>
       <c r="B82" s="6" t="inlineStr">
         <is>
-          <t>Managing the 1-39th branches of the sequested lands of German colonists at the Kholm-Volyn Department of Agriculture and State Property of Zhytomyr, Volyn Province</t>
+          <t>Управляючі 1-39-м відділеннями секвестрованих земель німців-колоністів при Холмсько-Волинському управлінні землеробства і державного майна м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C82" s="27" t="inlineStr">
@@ -3469,7 +3469,7 @@
       </c>
       <c r="B83" s="6" t="inlineStr">
         <is>
-          <t>Authorized Chairman of the Special Meeting for the Provision of Wood Fuel of Volyn Province Zhytomyr, Volyn Province</t>
+          <t>Уповноважений голови особливої наради по забезпеченню деревним паливом Волинської губернії м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C83" s="27" t="inlineStr">
@@ -3496,7 +3496,7 @@
       </c>
       <c r="B84" s="6" t="inlineStr">
         <is>
-          <t>Head of the Volyn-Podilsky Sand-Jar District of Zhytomyr, Volyn Province</t>
+          <t>Завідуючий Волинсько-Подільським піщано-яружним округом м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C84" s="27" t="inlineStr">
@@ -3523,7 +3523,7 @@
       </c>
       <c r="B85" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial in Peasant Affairs is a Zhytomyr, Volyn province</t>
+          <t>Волинське губернське у селянських справах присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C85" s="27" t="inlineStr">
@@ -3550,7 +3550,7 @@
       </c>
       <c r="B86" s="6" t="inlineStr">
         <is>
-          <t>Department of State Property of Radom, Kelets, Lublin, Sedletsky Provinces of the Main Department of Land Management and Agriculture in Radom, Radom Lips.</t>
+          <t>Управління державного майна Радомської, Келецької, Люблінської, Седлецької губерній Головного управління землевпорядкування і землеробства м. Радом, Радомської губ.</t>
         </is>
       </c>
       <c r="C86" s="27" t="inlineStr">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="B87" s="6" t="inlineStr">
         <is>
-          <t>Volyn State Chamber, Zhytomyr of Volyn Province</t>
+          <t>Волинська казенна палата, м. Житомир Волинської губернії</t>
         </is>
       </c>
       <c r="C87" s="27" t="inlineStr">
@@ -3604,7 +3604,7 @@
       </c>
       <c r="B88" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial District Committee of Zhytomyr, Volyn Province</t>
+          <t>Волинський губернський розпорядчий комітет м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C88" s="27" t="inlineStr">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="B89" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Excise Directorate of Zhytomyr, Volyn Province</t>
+          <t>Волинське губернське акцизне управління м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C89" s="27" t="inlineStr">
@@ -3658,7 +3658,7 @@
       </c>
       <c r="B90" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr County in Chinchi Affairs, Zhytomyr, Volyn Province.</t>
+          <t>Житомирське повітове у чиншових справах присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C90" s="27" t="inlineStr">
@@ -3685,7 +3685,7 @@
       </c>
       <c r="B91" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volynske county in the chin cases is present in Nov.-Volynsky, Volyn province</t>
+          <t>Новоград-Волинське повітове у чиншових справах присутствіє м. Нов.-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C91" s="27" t="inlineStr">
@@ -3712,7 +3712,7 @@
       </c>
       <c r="B92" s="6" t="inlineStr">
         <is>
-          <t>Ovruch county in the chin cases is present in Ovruch, Volyn province</t>
+          <t>Овруцьке повітове у чиншових справах присутствіє м. Овруч, Волинської губернії</t>
         </is>
       </c>
       <c r="C92" s="27" t="inlineStr">
@@ -3739,7 +3739,7 @@
       </c>
       <c r="B93" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr county leader of the nobility of Zhytomyr, Volyn province</t>
+          <t>Житомирський повітовий предводитель дворянства м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C93" s="27" t="inlineStr">
@@ -3766,7 +3766,7 @@
       </c>
       <c r="B94" s="6" t="inlineStr">
         <is>
-          <t>Ovruch county leader of the nobility of Zhytomyr. Volyn province</t>
+          <t>Овруцький повітовий предводитель дворянства м. Житомир. Волинської губернії</t>
         </is>
       </c>
       <c r="C94" s="27" t="inlineStr">
@@ -3793,7 +3793,7 @@
       </c>
       <c r="B95" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr-Orutz congress of world intermediaries of Zhytomyr, Volyn province</t>
+          <t>Житомирсько-Оруцький з'їзд мирових посередників м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C95" s="27" t="inlineStr">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="B96" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volyn-Rivensky Congress of Peace Medaries of Novograd-Volynskyi, Volyn Province</t>
+          <t>Новоград-Волинсько-Ровенський з'їзд мирових посередників м. Новоград-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C96" s="27" t="inlineStr">
@@ -3847,7 +3847,7 @@
       </c>
       <c r="B97" s="6" t="inlineStr">
         <is>
-          <t>The Medicament of the 2nd District of Zhytomyr County</t>
+          <t>Мировий посередник 2-ої дільниці Житомирського повіту</t>
         </is>
       </c>
       <c r="C97" s="27" t="inlineStr">
@@ -3874,7 +3874,7 @@
       </c>
       <c r="B98" s="6" t="inlineStr">
         <is>
-          <t>Volyn noble deputies of Zhytomyr, Volyn province</t>
+          <t>Волинські дворянські депутатські збори м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C98" s="27" t="inlineStr">
@@ -3901,7 +3901,7 @@
       </c>
       <c r="B99" s="6" t="inlineStr">
         <is>
-          <t>Volyn Diocesan School Council of Zhytomyr, Volyn Province</t>
+          <t>Волинська єпархіальна училищна рада м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C99" s="27" t="inlineStr">
@@ -3928,7 +3928,7 @@
       </c>
       <c r="B100" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Maker and Notary A. Mayan of Zhytomyr, Volyn Province</t>
+          <t>Житомирський маклер і нотаріус А. Майман м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C100" s="27" t="inlineStr">
@@ -3955,7 +3955,7 @@
       </c>
       <c r="B101" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Maker S. Kashperovsky Zhytomyr, Volyn Province</t>
+          <t>Житомирський маклер С. Кашперовський м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C101" s="27" t="inlineStr">
@@ -3982,7 +3982,7 @@
       </c>
       <c r="B102" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Maker and notary Z. Birstein, Zhytomyr, Volyn province</t>
+          <t>Житомирський маклер і нотаріус З. Бірштейн м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C102" s="27" t="inlineStr">
@@ -4009,7 +4009,7 @@
       </c>
       <c r="B103" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Maker and notary FI Muravyov, Zhytomyr, Volyn province</t>
+          <t>Житомирський маклер і нотаріус Ф. І. Муравйов м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C103" s="27" t="inlineStr">
@@ -4036,7 +4036,7 @@
       </c>
       <c r="B104" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Maker MP Zhnikroup Zhytomyr, Volyn Province</t>
+          <t>Житомирський маклер М. П. Жникрупа м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C104" s="27" t="inlineStr">
@@ -4063,7 +4063,7 @@
       </c>
       <c r="B105" s="6" t="inlineStr">
         <is>
-          <t>The Office of the Volyn Diocesan Bishop of Zhytomyr, Volyn Province</t>
+          <t>Канцелярія Волинського єпархіального архієрея м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C105" s="27" t="inlineStr">
@@ -4090,7 +4090,7 @@
       </c>
       <c r="B106" s="6" t="inlineStr">
         <is>
-          <t>Volyn Order of Public Guardians</t>
+          <t>Волинський приказ громадської опіки</t>
         </is>
       </c>
       <c r="C106" s="27" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="B107" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial in Zemsky and City Affairs is a Zhytomyr, Volyn province</t>
+          <t>Волинське губернське у земських та міських справах присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C107" s="27" t="inlineStr">
@@ -4144,7 +4144,7 @@
       </c>
       <c r="B108" s="6" t="inlineStr">
         <is>
-          <t>Baron De de-Duguar Ivan Maximilianovich</t>
+          <t>Барон де-Шодуар Іван Максиміліанович</t>
         </is>
       </c>
       <c r="C108" s="27" t="inlineStr">
@@ -4171,7 +4171,7 @@
       </c>
       <c r="B109" s="6" t="inlineStr">
         <is>
-          <t>Merchants Zhuravlev: Mykola Oleksiyovych, Vladimir, Nadiya Vladimirovna</t>
+          <t>Купці Журавльови:Микола Олексійович, Володимир Олексійович, Надія Володимирівна</t>
         </is>
       </c>
       <c r="C109" s="27" t="inlineStr">
@@ -4198,7 +4198,7 @@
       </c>
       <c r="B110" s="6" t="inlineStr">
         <is>
-          <t>Congress of Mary Judges of Zhytomyr Judicial and Mirory District of Zhytomyr</t>
+          <t>З'їзд мирових суддів Житомирського судово-мирового округу м. Житомир</t>
         </is>
       </c>
       <c r="C110" s="27" t="inlineStr">
@@ -4225,7 +4225,7 @@
       </c>
       <c r="B111" s="6" t="inlineStr">
         <is>
-          <t>The world judge of the 1st section of the Zhytomyr Judicial-Mira District</t>
+          <t>Мировий суддя 1-ої дільниці Житомирського судово-мирового округу</t>
         </is>
       </c>
       <c r="C111" s="27" t="inlineStr">
@@ -4252,7 +4252,7 @@
       </c>
       <c r="B112" s="6" t="inlineStr">
         <is>
-          <t>The Judge of the 2nd District of Zhytomyr Judiciary District</t>
+          <t>Мировий суддя 2-ої дільниці Житомирського судово-мирового округу</t>
         </is>
       </c>
       <c r="C112" s="27" t="inlineStr">
@@ -4279,7 +4279,7 @@
       </c>
       <c r="B113" s="6" t="inlineStr">
         <is>
-          <t>The Judge of the 3rd District of Zhytomyr Judicial District</t>
+          <t>Мировий суддя 3-ої дільниці Житомирського судово-мирового округу</t>
         </is>
       </c>
       <c r="C113" s="27" t="inlineStr">
@@ -4306,7 +4306,7 @@
       </c>
       <c r="B114" s="6" t="inlineStr">
         <is>
-          <t>The Judge of the 4th District District District</t>
+          <t>Мировий суддя 4-ої дільниці судово-мирового округу</t>
         </is>
       </c>
       <c r="C114" s="27" t="inlineStr">
@@ -4333,7 +4333,7 @@
       </c>
       <c r="B115" s="6" t="inlineStr">
         <is>
-          <t>Judge of the 5th District of the Judiciary District of Goroshka, Zhytomyr County</t>
+          <t>Мировий суддя 5-ої дільниці судово-мирового округу м. Горошки,Житомирського повіту</t>
         </is>
       </c>
       <c r="C115" s="27" t="inlineStr">
@@ -4360,7 +4360,7 @@
       </c>
       <c r="B116" s="6" t="inlineStr">
         <is>
-          <t>Judge of the 6th District of the Zhytomyr Judicial-Mirova District of Chudnov, Zhytomyr County</t>
+          <t>Мировий суддя 6-ої дільниці Житомирського судово-мирового округу м-ко Чуднів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C116" s="27" t="inlineStr">
@@ -4387,7 +4387,7 @@
       </c>
       <c r="B117" s="6" t="inlineStr">
         <is>
-          <t>Judge of the 7th Station</t>
+          <t>Мировий суддя 7-ої дільниці Житомирського судово-мирового округу м-ко Черняхів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C117" s="27" t="inlineStr">
@@ -4414,7 +4414,7 @@
       </c>
       <c r="B118" s="6" t="inlineStr">
         <is>
-          <t>Judge of the 8th District of Zhytomyr Judiciary District of Yanushpil, Zhytomyr County</t>
+          <t>Мировий суддя 8-ої дільниці Житомирського судово-мирового округу м-ко Янушпіль, Житомирського повіту</t>
         </is>
       </c>
       <c r="C118" s="27" t="inlineStr">
@@ -4441,7 +4441,7 @@
       </c>
       <c r="B119" s="6" t="inlineStr">
         <is>
-          <t>Upper Village Court at the 5th Am District of Zhytomyr Judiciary District</t>
+          <t>Верхній сільський суд при 5-й мировій дільниці Житомирського судово-мирового округу м-ко Горошки Житомирського повіту</t>
         </is>
       </c>
       <c r="C119" s="27" t="inlineStr">
@@ -4468,7 +4468,7 @@
       </c>
       <c r="B120" s="6" t="inlineStr">
         <is>
-          <t>The Upper Village Court at the 6th Am District</t>
+          <t>Верхній сільський суд при 6-й мировій дільниці Житомирського судово-мирового округу м-ко Чуднів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C120" s="27" t="inlineStr">
@@ -4495,7 +4495,7 @@
       </c>
       <c r="B121" s="6" t="inlineStr">
         <is>
-          <t>Lutsk-Zhytomyr Roman Catholic Spiritual Consistory of Zhytomyr, Volyn Province</t>
+          <t>Луцько-Житомирська римо-католицька духовна консисторія м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C121" s="27" t="inlineStr">
@@ -4522,7 +4522,7 @@
       </c>
       <c r="B122" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Branch of the State Bank of Zhytomyr, Volyn Province</t>
+          <t>Житомирське відділення Державного банку м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C122" s="27" t="inlineStr">
@@ -4549,7 +4549,7 @@
       </c>
       <c r="B123" s="6" t="inlineStr">
         <is>
-          <t>Volyn Branch of the Peasant Land Bank of Zhytomyr, Volyn Province</t>
+          <t>Волинське відділення селянського поземельного банку м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C123" s="27" t="inlineStr">
@@ -4576,7 +4576,7 @@
       </c>
       <c r="B124" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Zemsky Administration of Zhytomyr, Volyn Province</t>
+          <t>Волинська губернська земська управа м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C124" s="27" t="inlineStr">
@@ -4603,7 +4603,7 @@
       </c>
       <c r="B125" s="6" t="inlineStr">
         <is>
-          <t>Additional Judge of Zhytomyr Judicial and Mirova District of Zhytomyr, Volyn Province</t>
+          <t>Додатковий мировий суддя Житомирського судово-мирового округу м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C125" s="27" t="inlineStr">
@@ -4630,7 +4630,7 @@
       </c>
       <c r="B126" s="6" t="inlineStr">
         <is>
-          <t>Chyzhivska Solomo-cardboard and paper factory of the landowner Mezentsev Boris Sergeyevich village. Chizhivka, Nov.-Volyn County</t>
+          <t>Чижівська соломо-картонно-паперова фабрика поміщика Мезенцева Бориса Сергійовича с. Чижівка, Нов.-Волинського повіту</t>
         </is>
       </c>
       <c r="C126" s="27" t="inlineStr">
@@ -4657,7 +4657,7 @@
       </c>
       <c r="B127" s="6" t="inlineStr">
         <is>
-          <t>The Volyn Society of Khmelars in Zhytomyr, Volyn Province</t>
+          <t>Волинське товариство хмелярів м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C127" s="27" t="inlineStr">
@@ -4684,7 +4684,7 @@
       </c>
       <c r="B128" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr loan-savings companies of Khmelari Zhytomyr, Volyn province</t>
+          <t>Житомирське позичково-ощадне товариств хмелярів м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C128" s="27" t="inlineStr">
@@ -4711,7 +4711,7 @@
       </c>
       <c r="B129" s="6" t="inlineStr">
         <is>
-          <t>Central State Savings Cashier No. 124 of Zhytomyr Branch of the State Bank of Zhytomyr. Volyn province</t>
+          <t>Центральна державна ощадна каса № 124 Житомирського відділення Державного банку м. Житомир. Волинської губернії</t>
         </is>
       </c>
       <c r="C129" s="27" t="inlineStr">
@@ -4738,7 +4738,7 @@
       </c>
       <c r="B130" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr County Treasury. Zhytomyr (provincial) Treasury of Zhytomyr, Volyn Province</t>
+          <t>Житомирське повітове казначейство. Житомирське (губернське) казначейство м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C130" s="27" t="inlineStr">
@@ -4765,7 +4765,7 @@
       </c>
       <c r="B131" s="6" t="inlineStr">
         <is>
-          <t>State Savings Cashier No. 817 of the Zhytomyr Provincial Treasury of Zhytomyr, Volyn Province</t>
+          <t>Державна ощадна каса № 817 Житомирського губернського казначейства м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C131" s="27" t="inlineStr">
@@ -4792,7 +4792,7 @@
       </c>
       <c r="B132" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Cashier of Small Credit in Zhytomyr, Volyn Province</t>
+          <t>Волинська губернська каса дрібного кредиту м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C132" s="27" t="inlineStr">
@@ -4819,7 +4819,7 @@
       </c>
       <c r="B133" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Mutual Credit Society of Zhytomyr, Volyn Province</t>
+          <t>Житомирське товариство взаємного кредиту м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C133" s="27" t="inlineStr">
@@ -4846,7 +4846,7 @@
       </c>
       <c r="B134" s="6" t="inlineStr">
         <is>
-          <t>Volyn Branch of the Azov-Don Commercial Bank of Zhytomyr, Volyn Province</t>
+          <t>Волинське відділення Азово-Донського комерційного банку м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C134" s="27" t="inlineStr">
@@ -4873,7 +4873,7 @@
       </c>
       <c r="B135" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Agency of the Salamandra Insurance Society, Zhytomyr, Volyn Province</t>
+          <t>Житомирське агенство страхового товариства «Саламандра» м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C135" s="27" t="inlineStr">
@@ -4900,7 +4900,7 @@
       </c>
       <c r="B136" s="6" t="inlineStr">
         <is>
-          <t>Ship forestry of the Volyn Chamber of State Property of Zhytomyr, Volyn Province</t>
+          <t>Корабельне лісництво Волинської палати державного майна м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C136" s="27" t="inlineStr">
@@ -4927,7 +4927,7 @@
       </c>
       <c r="B137" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr-Ovrutsk district in the chin cases is present in Zhytomyr, Volyn province</t>
+          <t>Житомирсько-Овруцьке повітове у чиншових справах присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C137" s="27" t="inlineStr">
@@ -4954,7 +4954,7 @@
       </c>
       <c r="B138" s="6" t="inlineStr">
         <is>
-          <t>Goroshkivsky Postal and Telegraph department</t>
+          <t>Горошківське поштово-телеграфне відділення м-ко Горошки, Житомирського повіту</t>
         </is>
       </c>
       <c r="C138" s="27" t="inlineStr">
@@ -4981,7 +4981,7 @@
       </c>
       <c r="B139" s="6" t="inlineStr">
         <is>
-          <t>Statistical Bureau of the Volyn Provincial Zemsky Directorate of Zhytomyr, Volyn Province</t>
+          <t>Статистичне бюро Волинської губернської земської управи м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C139" s="27" t="inlineStr">
@@ -5008,7 +5008,7 @@
       </c>
       <c r="B140" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr postal and telegraph office of Zhytomyr, Volyn province</t>
+          <t>Житомирська поштово-телеграфна контора м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C140" s="27" t="inlineStr">
@@ -5035,7 +5035,7 @@
       </c>
       <c r="B141" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Teachers' Seminary Zhytomyr, Volyn Province</t>
+          <t>Житомирська учительська семінарія м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C141" s="27" t="inlineStr">
@@ -5062,7 +5062,7 @@
       </c>
       <c r="B142" s="6" t="inlineStr">
         <is>
-          <t>Radomysl Fund-Telegraph Office of Radomysl, Kyiv Province</t>
+          <t>Радомисльська коштово-телеграфна контора м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C142" s="27" t="inlineStr">
@@ -5089,7 +5089,7 @@
       </c>
       <c r="B143" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Land Management Commission of Zhytomyr, Volyn Province</t>
+          <t>Волинська губернська землевпорядна комісія м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C143" s="27" t="inlineStr">
@@ -5116,7 +5116,7 @@
       </c>
       <c r="B144" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Forestry of the Volyn Chamber of State Property of Zhytomyr, Volyn Province</t>
+          <t>Житомирське лісництво Волинської палати державного майна м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C144" s="27" t="inlineStr">
@@ -5143,7 +5143,7 @@
       </c>
       <c r="B145" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Land College of Zhytomyr, Volyn Province</t>
+          <t>Житомирське землемірне училище м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C145" s="27" t="inlineStr">
@@ -5170,7 +5170,7 @@
       </c>
       <c r="B146" s="6" t="inlineStr">
         <is>
-          <t>Stanishevsky forestry of Volyn Department of Agriculture and State Property Stanyshivka, Zhytomyr County, Volyn Province</t>
+          <t>Станишівське лісництво Волинського управління землеробства та державного майна с. Станишівка, Житомирський повіт, Волинської губернії</t>
         </is>
       </c>
       <c r="C146" s="27" t="inlineStr">
@@ -5197,7 +5197,7 @@
       </c>
       <c r="B147" s="6" t="inlineStr">
         <is>
-          <t>The Volyn Provincial Recruitian presence is Zhytomyr, Volyn province</t>
+          <t>Волинське губернське рекрутське присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C147" s="27" t="inlineStr">
@@ -5224,7 +5224,7 @@
       </c>
       <c r="B148" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv Public Maker and Notary Chaim Volkenstein M-Kok Berdychiv, Zhytomyr County</t>
+          <t>Бердичівький публічний маклер та нотаріус Хаїм Волкенштейн м-ко Бердичів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C148" s="27" t="inlineStr">
@@ -5251,7 +5251,7 @@
       </c>
       <c r="B149" s="6" t="inlineStr">
         <is>
-          <t>Berdichevsky Maker and Notary Moshko Kudysh Mr. Berdychiv, Zhytomyr County</t>
+          <t>Бердичівський маклер та нотаріус Мошко Кудиш м-ко Бердичів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C149" s="27" t="inlineStr">
@@ -5278,7 +5278,7 @@
       </c>
       <c r="B150" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv Public Notary Pinkhos Weinstein M-ko Berdychiv, Zhytomyr County</t>
+          <t>Бердичівський публічний нотаріус Пінхос Вайнштейн м-ко Бердичів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C150" s="27" t="inlineStr">
@@ -5305,7 +5305,7 @@
       </c>
       <c r="B151" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv Public Notary Gregory Leonson M-Kok Berdychiv, Zhytomyr County</t>
+          <t>Бердичівський публічний нотаріус Григорій Леонсон м-ко Бердичів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C151" s="27" t="inlineStr">
@@ -5332,7 +5332,7 @@
       </c>
       <c r="B152" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial for Industrial Tax is a Zhytomyr, Volyn province</t>
+          <t>Волинське губернське по промисловому податку присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C152" s="27" t="inlineStr">
@@ -5359,7 +5359,7 @@
       </c>
       <c r="B153" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volynske in Chinshev's affairs is present in Novograd-Volynskyi, Volyn province</t>
+          <t>Новоград-Волинське по чиншевим справам присутствіє м. Новоград-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C153" s="27" t="inlineStr">
@@ -5386,7 +5386,7 @@
       </c>
       <c r="B154" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr City Tax is present in Zhytomyr, Volyn province</t>
+          <t>Житомирське міське по квартирному податку присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C154" s="27" t="inlineStr">
@@ -5413,7 +5413,7 @@
       </c>
       <c r="B155" s="6" t="inlineStr">
         <is>
-          <t>The Medicament of the 2nd District of Novograd-Volyn County</t>
+          <t>Мировий посередник 2-ої дільниці Новоград-Волинського повіту</t>
         </is>
       </c>
       <c r="C155" s="27" t="inlineStr"/>
@@ -5436,7 +5436,7 @@
       </c>
       <c r="B156" s="6" t="inlineStr">
         <is>
-          <t>Peaceful mediator of the 2nd section of Novograd-Volyn district, Novograd-Volyn Volyn province</t>
+          <t>Мировий посередник 2-ї дільниці Новоград-Волинського повіту, м. Новоград-Волинський Волинської губернії</t>
         </is>
       </c>
       <c r="C156" s="27" t="inlineStr">
@@ -5463,7 +5463,7 @@
       </c>
       <c r="B157" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Women's Gymnasium NV Ovsyannikova, Zhytomyr, Volyn Province</t>
+          <t>Житомирська жіноча гімназія Н. В. Овсянникової м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C157" s="27" t="inlineStr">
@@ -5490,7 +5490,7 @@
       </c>
       <c r="B158" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volyn Men's Gymnasium of Novograd-Volynsky, Volyn Province</t>
+          <t>Новоград-Волинська чоловіча гімназія м. Новоград-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C158" s="27" t="inlineStr">
@@ -5517,7 +5517,7 @@
       </c>
       <c r="B159" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr 1st higher-laid male school of Zhytomyr, Volyn province</t>
+          <t>Житомирське 1-ше вище-початкове чоловіче училище м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C159" s="27" t="inlineStr">
@@ -5544,7 +5544,7 @@
       </c>
       <c r="B160" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr two-year pedagogical courses at the Zhytomyr First Higher Men's School of Zhytomyr, Volyn Province</t>
+          <t>Житомирські дворічні педагогічні курси при Житомирському Першому вище-початковому чоловічому училищі м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C160" s="27" t="inlineStr">
@@ -5571,7 +5571,7 @@
       </c>
       <c r="B161" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Agemir of Zhytomyr, Volyn Province</t>
+          <t>Волинський губернський землемір м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C161" s="27" t="inlineStr">
@@ -5598,7 +5598,7 @@
       </c>
       <c r="B162" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr State Cleansing Composition №1 of Volyn Provincial Excise Department of Zhytomyr, Volyn Province</t>
+          <t>Житомирський казенний очисний склад №1 Волинського губернського акцизного управління м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C162" s="27" t="inlineStr">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="B163" s="6" t="inlineStr">
         <is>
-          <t>Lubarsky Tales of Cleaning No. 2 of Volyn Provincial Excise Department</t>
+          <t>Любарський казенний очисний склад №2 Волинського губернського акцизного управління м-ко Любар, Нов.-Волинського повіту</t>
         </is>
       </c>
       <c r="C163" s="27" t="inlineStr">
@@ -5652,7 +5652,7 @@
       </c>
       <c r="B164" s="6" t="inlineStr">
         <is>
-          <t>Charity monasteries of the Volyn Diocese of Zhytomyr, Volyn Province</t>
+          <t>Благочинний монастирів Волинської єпархії м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C164" s="27" t="inlineStr">
@@ -5679,7 +5679,7 @@
       </c>
       <c r="B165" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial on Real Estate Tax is present in Zhytomyr, Volyn province</t>
+          <t>Волинське губернське по податку з нерухомого майна присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C165" s="27" t="inlineStr">
@@ -5706,7 +5706,7 @@
       </c>
       <c r="B166" s="6" t="inlineStr">
         <is>
-          <t>Kodnyansk Postal and Telegraph State Savings Cashier №14 M-Kodnya, Zhytomyr County</t>
+          <t>Коднянська поштово-телеграфна державна ощадна каса №14 м-ко Кодня, Житомирського повіту</t>
         </is>
       </c>
       <c r="C166" s="27" t="inlineStr">
@@ -5733,7 +5733,7 @@
       </c>
       <c r="B167" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr County Zemsky Administration of Zhytomyr, Volyn Province</t>
+          <t>Житомирська повітова земська управа м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C167" s="27" t="inlineStr">
@@ -5760,7 +5760,7 @@
       </c>
       <c r="B168" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Commercial and Slavic Court of Zhytomyr, Volyn Province</t>
+          <t>Житомирський торгово-словесний суд м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C168" s="27" t="inlineStr">
@@ -5787,7 +5787,7 @@
       </c>
       <c r="B169" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Commercial Bank of Zhytomyr, Volyn Province</t>
+          <t>Житомирський комерційний банк м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C169" s="27" t="inlineStr">
@@ -5814,7 +5814,7 @@
       </c>
       <c r="B170" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Assay Chamber of Zhytomyr, Volyn Province</t>
+          <t>Житомирська пробірна палата м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C170" s="27" t="inlineStr">
@@ -5841,7 +5841,7 @@
       </c>
       <c r="B171" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Union of Credit and Loan-Savings Societies of Zhytomyr, Volyn Province</t>
+          <t>Житомирська спілка кредитних та позичково-ощадних товариств м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C171" s="27" t="inlineStr">
@@ -5868,7 +5868,7 @@
       </c>
       <c r="B172" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr County Recruary is present in Zhytomyr, Volyn province</t>
+          <t>Житомирське повітове рекрутьке присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C172" s="27" t="inlineStr">
@@ -5895,7 +5895,7 @@
       </c>
       <c r="B173" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Committee of the All -Russian Union of Cities of Assistance to sick and wounded soldiers of Zhytomyr, Volyn province</t>
+          <t>Житомирський комітет Всеросійського Союзу міст допомоги хворим та пораненим воїнам м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C173" s="27" t="inlineStr">
@@ -5922,7 +5922,7 @@
       </c>
       <c r="B174" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr County on real estate tax is present in Zhytomyr, Volyn province</t>
+          <t>Житомирське повітове по податку з нерухомого майна присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C174" s="27" t="inlineStr">
@@ -5949,7 +5949,7 @@
       </c>
       <c r="B175" s="6" t="inlineStr">
         <is>
-          <t>Luginsky forestry of Lugini, Ovruch district, Volyn province</t>
+          <t>Лугинське лісництво м-ко Лугини, Овруцького повіту, Волинської губернії</t>
         </is>
       </c>
       <c r="C175" s="27" t="inlineStr">
@@ -5976,7 +5976,7 @@
       </c>
       <c r="B176" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volyn County Tomb. Novograd-Volynskyi, Volyn province</t>
+          <t>Новоград-Волинське повітове розкладкове присутствіє м. Новоград-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C176" s="27" t="inlineStr">
@@ -6003,7 +6003,7 @@
       </c>
       <c r="B177" s="6" t="inlineStr">
         <is>
-          <t>Ovruch County Land Management Commission of Ovruch, Volyn Province</t>
+          <t>Овруцька повітова землевпорядна комісія м. Овруч, Волинської губернії</t>
         </is>
       </c>
       <c r="C177" s="27" t="inlineStr">
@@ -6030,7 +6030,7 @@
       </c>
       <c r="B178" s="6" t="inlineStr">
         <is>
-          <t>Ovruch City Two -Class School of Ovruch, Volyn Province</t>
+          <t>Овруцьке міське двокласне училище м. Овруч, Волинської губернії</t>
         </is>
       </c>
       <c r="C178" s="27" t="inlineStr">
@@ -6057,7 +6057,7 @@
       </c>
       <c r="B179" s="6" t="inlineStr">
         <is>
-          <t>Ovruch forestry of Ovruch, Volyn province</t>
+          <t>Овруцьке лісництво м. Овруч, Волинської губернії</t>
         </is>
       </c>
       <c r="C179" s="27" t="inlineStr">
@@ -6084,7 +6084,7 @@
       </c>
       <c r="B180" s="6" t="inlineStr">
         <is>
-          <t>The Ovruch County Recruary presence is Ovruch, Volyn Province</t>
+          <t>Овруцьке повітове рекрутське присутствіє м. Овруч, Волинської губернії</t>
         </is>
       </c>
       <c r="C180" s="27" t="inlineStr">
@@ -6111,7 +6111,7 @@
       </c>
       <c r="B181" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr County Tomb in Zhytomyr, Volyn Province</t>
+          <t>Житомирське повітове розкладкове присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C181" s="27" t="inlineStr">
@@ -6138,7 +6138,7 @@
       </c>
       <c r="B182" s="6" t="inlineStr">
         <is>
-          <t>Radomysl County Court of Radomysl, Kyiv Province</t>
+          <t>Радомисльський повітовий суд м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C182" s="27" t="inlineStr">
@@ -6165,7 +6165,7 @@
       </c>
       <c r="B183" s="6" t="inlineStr">
         <is>
-          <t>Radomysl County Land Management Commission of Radomysl, Kyiv Province</t>
+          <t>Радомисльська повітова землевпорядна комісія м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C183" s="27" t="inlineStr">
@@ -6192,7 +6192,7 @@
       </c>
       <c r="B184" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Lower Zemsky Court of Zhytomyr, Volyn Province</t>
+          <t>Житомирський нижній земський суд м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C184" s="27" t="inlineStr">
@@ -6219,7 +6219,7 @@
       </c>
       <c r="B185" s="6" t="inlineStr">
         <is>
-          <t>Chernyakhiv postal and telegraph office of Chernyakhiv, Zhytomyr County</t>
+          <t>Черняхівська поштово-телеграфна контора м-ко Черняхів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C185" s="27" t="inlineStr">
@@ -6246,7 +6246,7 @@
       </c>
       <c r="B186" s="6" t="inlineStr">
         <is>
-          <t>The 3rd part of the 4th state of Zhytomyr, Volyn province</t>
+          <t>Пристав 3-ої частини 4-го стану м. Житомир, Волинськї губернії</t>
         </is>
       </c>
       <c r="C186" s="27" t="inlineStr">
@@ -6273,7 +6273,7 @@
       </c>
       <c r="B187" s="6" t="inlineStr">
         <is>
-          <t>Office of Zhytomyr County Military Chief of Zhytomyr, Volyn Province</t>
+          <t>Управління Житомирського повітового військового начальника м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C187" s="27" t="inlineStr">
@@ -6300,7 +6300,7 @@
       </c>
       <c r="B188" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Congress Competitive Court of Zhytomyr, Volyn Province</t>
+          <t>Житомирський з'їздовий конкурсний суд м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C188" s="27" t="inlineStr">
@@ -6327,7 +6327,7 @@
       </c>
       <c r="B189" s="6" t="inlineStr">
         <is>
-          <t>Society of Ivankivsky Sugar Broad Plant Ivankiv, Zhytomyr county</t>
+          <t>Товариство Іванківського цукробурякового заводу с. Іванків, Житомирського повіту</t>
         </is>
       </c>
       <c r="C189" s="27" t="inlineStr">
@@ -6354,7 +6354,7 @@
       </c>
       <c r="B190" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Magistrate in Zhytomyr, Volyn Province</t>
+          <t>Волинський губернський магістрат м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C190" s="27" t="inlineStr">
@@ -6381,7 +6381,7 @@
       </c>
       <c r="B191" s="6" t="inlineStr">
         <is>
-          <t>Volyn Upper Comraction of Zhytomyr, Volyn Province</t>
+          <t>Волинська верхня розправа м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C191" s="27" t="inlineStr">
@@ -6408,7 +6408,7 @@
       </c>
       <c r="B192" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Political Meister of Zhytomyr, Volyn Province</t>
+          <t>Житомирський поліцмейстер м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C192" s="27" t="inlineStr">
@@ -6435,7 +6435,7 @@
       </c>
       <c r="B193" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial in Affairs of Society and Union is a presence of Zhytomyr, Volyn province</t>
+          <t>Волинське губернське у справах про товариства та союза присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C193" s="27" t="inlineStr">
@@ -6462,7 +6462,7 @@
       </c>
       <c r="B194" s="6" t="inlineStr">
         <is>
-          <t>Volyn provincial leader of the nobility of Zhytomyr, Volyn province</t>
+          <t>Волинський губернський предводитель дворянства м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C194" s="27" t="inlineStr">
@@ -6489,7 +6489,7 @@
       </c>
       <c r="B195" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volyn county from military service is present in Novograd-Volynsky, Volyn province</t>
+          <t>Новоград-Волинське повітове з військової повинності присутствіє м. Новоград-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C195" s="27" t="inlineStr">
@@ -6516,7 +6516,7 @@
       </c>
       <c r="B196" s="6" t="inlineStr">
         <is>
-          <t>The sub -inspector of Zhytomyr district Zhytomyr, Volyn province</t>
+          <t>Податний інспектор Житомирського повіту м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C196" s="27" t="inlineStr">
@@ -6543,7 +6543,7 @@
       </c>
       <c r="B197" s="6" t="inlineStr">
         <is>
-          <t>The sub-inspector of the 1st section of Zhytomyr County</t>
+          <t>Податний інспектор 1-ої дільниці Житомирськго повіту</t>
         </is>
       </c>
       <c r="C197" s="27" t="inlineStr">
@@ -6570,7 +6570,7 @@
       </c>
       <c r="B198" s="6" t="inlineStr">
         <is>
-          <t>The sub-inspector of the 2nd section of Zhytomyr County</t>
+          <t>Податний інспектор 2-ої дільниці Житомирського повіту</t>
         </is>
       </c>
       <c r="C198" s="27" t="inlineStr">
@@ -6597,7 +6597,7 @@
       </c>
       <c r="B199" s="6" t="inlineStr">
         <is>
-          <t>Subject Inspector of Zhytomyr, Zhytomyr, Volyn Province</t>
+          <t>Податний інспектор м. Житомир, м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C199" s="27" t="inlineStr">
@@ -6624,7 +6624,7 @@
       </c>
       <c r="B200" s="6" t="inlineStr">
         <is>
-          <t>The sub-inspector of the 1st section of the city of Zhytomyr Zhytomyr, Volyn province</t>
+          <t>Податний інспектор 1-ої дільниці міста Житомира м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C200" s="27" t="inlineStr">
@@ -6651,7 +6651,7 @@
       </c>
       <c r="B201" s="6" t="inlineStr">
         <is>
-          <t>The sub-inspector of the 2nd section of Zhytomyr, Zhytomyr, Volyn province</t>
+          <t>Податний інспектор 2-ої дільниці м. Житомир, м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C201" s="27" t="inlineStr">
@@ -6678,7 +6678,7 @@
       </c>
       <c r="B202" s="6" t="inlineStr">
         <is>
-          <t>The sub-inspector of the 3rd section of the city of Zhytomyr, Zhytomyr, Volyn province</t>
+          <t>Податний інспектор 3-ої дільниці міста Житомира, м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C202" s="27" t="inlineStr">
@@ -6705,7 +6705,7 @@
       </c>
       <c r="B203" s="6" t="inlineStr">
         <is>
-          <t>The sub-inspector of the 4th section of the city of Zhytomyr Zhytomyr, Volyn province</t>
+          <t>Податний інспектор 4-ої дільниці міста Житомира м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C203" s="27" t="inlineStr">
@@ -6732,7 +6732,7 @@
       </c>
       <c r="B204" s="6" t="inlineStr">
         <is>
-          <t>Ovruch spiritual rule of Ovruch, Volyn province</t>
+          <t>Овруцьке духовне правління м. Овруч, Волинської губернії</t>
         </is>
       </c>
       <c r="C204" s="27" t="inlineStr">
@@ -6759,7 +6759,7 @@
       </c>
       <c r="B205" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr spiritual rule of Zhytomyr, Volyn province</t>
+          <t>Житомирське духовне правління м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C205" s="27" t="inlineStr">
@@ -6786,7 +6786,7 @@
       </c>
       <c r="B206" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volyn spiritual rule of Novograd-Volyn Volyn province</t>
+          <t>Новоград-Волинське духовне правління м. Новоград-Волинський Волинської губернії</t>
         </is>
       </c>
       <c r="C206" s="27" t="inlineStr">
@@ -6813,7 +6813,7 @@
       </c>
       <c r="B207" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr City Laming Aids Zhytomyr, Volyn Province</t>
+          <t>Житомирське міське розкладкове присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C207" s="27" t="inlineStr">
@@ -6840,7 +6840,7 @@
       </c>
       <c r="B208" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr city real estate tax is present in Zhytomyr, Volyn province</t>
+          <t>Житомирське міське по податку з нерухомого майна присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C208" s="27" t="inlineStr">
@@ -6867,7 +6867,7 @@
       </c>
       <c r="B209" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr boarding house of noble girls in Zhytomyr, Volyn province</t>
+          <t>Житомирський пансіон шляхетних дівчат м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C209" s="27" t="inlineStr">
@@ -6894,7 +6894,7 @@
       </c>
       <c r="B210" s="6" t="inlineStr">
         <is>
-          <t>Volyn Prosecutor of Zhytomyr, Volyn Province</t>
+          <t>Волинський губернський прокурор м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C210" s="27" t="inlineStr">
@@ -6921,7 +6921,7 @@
       </c>
       <c r="B211" s="6" t="inlineStr">
         <is>
-          <t>The sub-inspector of Novograd-Volyn district of Novograd-Volynsky, Volyn province</t>
+          <t>Податний інспектор Новоград-Волинського повіту м. Новоград-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C211" s="27" t="inlineStr">
@@ -6948,7 +6948,7 @@
       </c>
       <c r="B212" s="6" t="inlineStr">
         <is>
-          <t>The sub-inspector of the 1st district of Novograd-Volyn district of Novograd-Volynskyi, Volyn province</t>
+          <t>Податний інспектор 1-ої дільниці Новоград-Волинського повіту м. Новоград-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C212" s="27" t="inlineStr">
@@ -6975,7 +6975,7 @@
       </c>
       <c r="B213" s="6" t="inlineStr">
         <is>
-          <t>Government agronomist of Volyn province of Zhytomyr, Volyn province</t>
+          <t>Урядовий агроном Волинської губернії м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C213" s="27" t="inlineStr">
@@ -7002,7 +7002,7 @@
       </c>
       <c r="B214" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volynske Temporary Recruary presence is the city of Novograd-Volynsky, Volyn province</t>
+          <t>Новоград-Волинське тимчасове рекрутське присутствіє м. Новоград-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C214" s="27" t="inlineStr">
@@ -7029,7 +7029,7 @@
       </c>
       <c r="B215" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Jewish Teachers' Institute of Zhytomyr, Volyn Province</t>
+          <t>Житомирський єврейський учительський інститут м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C215" s="27" t="inlineStr">
@@ -7056,7 +7056,7 @@
       </c>
       <c r="B216" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Jewish State Town School of the 1st category of Zhytomyr, Volyn province</t>
+          <t>Житомирське єврейське казенне училище 1-го розряду м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C216" s="27" t="inlineStr">
@@ -7083,7 +7083,7 @@
       </c>
       <c r="B217" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Committee on the Migration of Jews of Zhytomyr, Volyn Province</t>
+          <t>Волинський губернський комітет по переселенню євреїв м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C217" s="27" t="inlineStr">
@@ -7110,7 +7110,7 @@
       </c>
       <c r="B218" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Jewish School Commission of Zhytomyr, Volyn Province</t>
+          <t>Волинська губернська єврейська училищна комісія м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C218" s="27" t="inlineStr">
@@ -7137,7 +7137,7 @@
       </c>
       <c r="B219" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Rabin College of Zhytomyr, Volyn Province</t>
+          <t>Житомирське рабинське училище м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C219" s="27" t="inlineStr">
@@ -7164,7 +7164,7 @@
       </c>
       <c r="B220" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr two -class Jewish elementary school of Zhytomyr, Volyn province</t>
+          <t>Житомирське двокласне єврейське початкове училище м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C220" s="27" t="inlineStr">
@@ -7191,7 +7191,7 @@
       </c>
       <c r="B221" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Jewish Public School "Talmud-Ttor" Zhytomyr, Volyn Province</t>
+          <t>Житомирське єврейське громадське училище «Талмуд-Тора» м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C221" s="27" t="inlineStr">
@@ -7218,7 +7218,7 @@
       </c>
       <c r="B222" s="6" t="inlineStr">
         <is>
-          <t>Vice Dekan, Zhytomyr Department of Zhytomyr, Volyn Province</t>
+          <t>Віце-декан Житомирської кафедри м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C222" s="27" t="inlineStr">
@@ -7245,7 +7245,7 @@
       </c>
       <c r="B223" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr County Dean of Zhytomyr, Volyn Province</t>
+          <t>Житомирський повітовий декан м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C223" s="27" t="inlineStr">
@@ -7272,7 +7272,7 @@
       </c>
       <c r="B224" s="6" t="inlineStr">
         <is>
-          <t>Raygorod Postal and Telegraph Branch</t>
+          <t>Райгородське поштово-телеграфне відділення м-ко Райгородок, Житомирського повіту</t>
         </is>
       </c>
       <c r="C224" s="27" t="inlineStr">
@@ -7299,7 +7299,7 @@
       </c>
       <c r="B225" s="6" t="inlineStr">
         <is>
-          <t>Maryatyn's one -class public school of the village. Maryatin, Ovruch County</t>
+          <t>Мар'ятинське однокласне народне училище с. Мар'ятин, Овруцького повіту</t>
         </is>
       </c>
       <c r="C225" s="27" t="inlineStr">
@@ -7326,7 +7326,7 @@
       </c>
       <c r="B226" s="6" t="inlineStr">
         <is>
-          <t>Chudnivsky city on real estate tax is present in the miracle, Zhytomyr district, Volyn province</t>
+          <t>Чуднівське міське по податку з нерухомого майна присутствіє м-ко Чуднів, Житомирського повіту, Волинської губернії</t>
         </is>
       </c>
       <c r="C226" s="27" t="inlineStr">
@@ -7353,7 +7353,7 @@
       </c>
       <c r="B227" s="6" t="inlineStr">
         <is>
-          <t>Chernyakhiv city on real estate tax is present in Chernyakhiv, Zhytomyr county</t>
+          <t>Черняхівське міське по податку з нерухомого майна  присутствіє м-ко Черняхів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C227" s="27" t="inlineStr">
@@ -7380,7 +7380,7 @@
       </c>
       <c r="B228" s="6" t="inlineStr">
         <is>
-          <t>The Volyn Provincial Church-Construction is Zhytomyr, Volyn Province</t>
+          <t>Волинське губернське церковно-будівельне присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C228" s="27" t="inlineStr">
@@ -7407,7 +7407,7 @@
       </c>
       <c r="B229" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provisional Propinal Commission of Zhytomyr, Volyn Province</t>
+          <t>Волинська тимчасова пропінаційна комісія м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C229" s="27" t="inlineStr">
@@ -7434,7 +7434,7 @@
       </c>
       <c r="B230" s="6" t="inlineStr">
         <is>
-          <t>Kutuziv Postal and Telegraph Office</t>
+          <t>Кутузівська поштово-телеграфна контора м-ко Кутузхове Житомирського повіту</t>
         </is>
       </c>
       <c r="C230" s="27" t="inlineStr">
@@ -7461,7 +7461,7 @@
       </c>
       <c r="B231" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr County College of Zhytomyr, Volyn Province</t>
+          <t>Житомирське повітове училище м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C231" s="27" t="inlineStr">
@@ -7488,7 +7488,7 @@
       </c>
       <c r="B232" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Noble Committee in Peasant Affairs of Zhytomyr, Volyn Province</t>
+          <t>Волинський губернський дворянський комітет у селянських справах м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C232" s="27" t="inlineStr">
@@ -7515,7 +7515,7 @@
       </c>
       <c r="B233" s="6" t="inlineStr">
         <is>
-          <t>The Church of Zhytomyr Goddivisions of Zhytomyr, Volyn Province</t>
+          <t>Церква Житомирських богоугодних закладів м. Житомир, Волинськї губернії</t>
         </is>
       </c>
       <c r="C233" s="27" t="inlineStr">
@@ -7542,7 +7542,7 @@
       </c>
       <c r="B234" s="6" t="inlineStr">
         <is>
-          <t>Volyn united on ensuring the life of the Orthodox clergy and in the peasant affairs there is Zhytomyr, Volyn province</t>
+          <t>Волинське об'єднане по забезпеченню побуту православного духовенства і у селянських справах присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C234" s="27" t="inlineStr">
@@ -7569,7 +7569,7 @@
       </c>
       <c r="B235" s="6" t="inlineStr">
         <is>
-          <t>Volyn Diocesan Audit Committee of Zhytomyr, Volyn Province</t>
+          <t>Волинський єпархіальний ревізійний комітет м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C235" s="27" t="inlineStr">
@@ -7596,7 +7596,7 @@
       </c>
       <c r="B236" s="6" t="inlineStr">
         <is>
-          <t>Lithuanian Greek-Uniate Spiritual Consistory</t>
+          <t>Литовська греко-уніатська духовна консисторія</t>
         </is>
       </c>
       <c r="C236" s="27" t="inlineStr">
@@ -7623,7 +7623,7 @@
       </c>
       <c r="B237" s="6" t="inlineStr">
         <is>
-          <t>Ovruch City Hospital in Ovruch. Volyn province</t>
+          <t>Овруцька міська лікарня м. Овруч. Волинської губернії</t>
         </is>
       </c>
       <c r="C237" s="27" t="inlineStr">
@@ -7650,7 +7650,7 @@
       </c>
       <c r="B238" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Orphan Court of Zhytomyr, Volyn Province</t>
+          <t>Житомирський сирітський суд м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C238" s="27" t="inlineStr">
@@ -7677,7 +7677,7 @@
       </c>
       <c r="B239" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Noble Assembly of Zhytomyr, Volyn Province</t>
+          <t>Житомирське благородне зібрання м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C239" s="27" t="inlineStr">
@@ -7704,7 +7704,7 @@
       </c>
       <c r="B240" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Committee for Consideration and Compilation of Inventory Descriptions</t>
+          <t>Волинський губернський комітет з розгляду та складання інвентарних описів поміщицьких маєтків м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C240" s="27" t="inlineStr">
@@ -7731,7 +7731,7 @@
       </c>
       <c r="B241" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr county from military service is present in Zhytomyr, Volyn province</t>
+          <t>Житомирське повітове з військової повинності присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C241" s="27" t="inlineStr">
@@ -7758,7 +7758,7 @@
       </c>
       <c r="B242" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Postal and Telegraph Office of Zhytomyr</t>
+          <t>Волинська губернська поштово-телеграфна контора м. Житомир</t>
         </is>
       </c>
       <c r="C242" s="27" t="inlineStr">
@@ -7785,7 +7785,7 @@
       </c>
       <c r="B243" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Cathedral of Zhytomyr, Volyn Province</t>
+          <t>Житомирський кафедральний собор м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C243" s="27" t="inlineStr">
@@ -7812,7 +7812,7 @@
       </c>
       <c r="B244" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial for Military Military Military Military Military Military Military Military Military, Volyn Province</t>
+          <t>Волинське губернське з військової повинності присутствіє м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C244" s="27" t="inlineStr">
@@ -7839,7 +7839,7 @@
       </c>
       <c r="B245" s="6" t="inlineStr">
         <is>
-          <t>Volyn Diocesan Administration of Zhytomyr, Volyn Province</t>
+          <t>Волинське єпархіальне управління м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C245" s="27" t="inlineStr">
@@ -7866,7 +7866,7 @@
       </c>
       <c r="B246" s="6" t="inlineStr">
         <is>
-          <t>Ovruch Lustration Commission of Ovruch, Volyn Province</t>
+          <t>Овруцька люстраційна комісія м. Овруч, Волинської губернії</t>
         </is>
       </c>
       <c r="C246" s="27" t="inlineStr">
@@ -7893,7 +7893,7 @@
       </c>
       <c r="B247" s="6" t="inlineStr">
         <is>
-          <t>Volyn-Zhytomyr Episcope of Zhytomyr, Volyn Province</t>
+          <t>Волинсько-Житомирський єпіскоп м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C247" s="27" t="inlineStr">
@@ -7920,7 +7920,7 @@
       </c>
       <c r="B248" s="6" t="inlineStr">
         <is>
-          <t>Lutsk-Zhytomyr Catholic Theological Seminary of Zhytomyr, Volyn Province</t>
+          <t>Луцько-Житомирська католицька духовна семінарія м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C248" s="27" t="inlineStr">
@@ -7947,7 +7947,7 @@
       </c>
       <c r="B249" s="6" t="inlineStr">
         <is>
-          <t>Stremigorod District Government of the village. Stremigorod, Radomysl county</t>
+          <t>Стремигородське волосне правління с. Стремигород, Радомисльського повіту</t>
         </is>
       </c>
       <c r="C249" s="27" t="inlineStr">
@@ -7974,7 +7974,7 @@
       </c>
       <c r="B250" s="6" t="inlineStr">
         <is>
-          <t>Pinyazevitsky District Government with Pinyazevichi, Radomysl County</t>
+          <t>Пинязевицьке волосне правління с Пинязевичі, Радомисльського повіту</t>
         </is>
       </c>
       <c r="C250" s="27" t="inlineStr">
@@ -8001,7 +8001,7 @@
       </c>
       <c r="B251" s="6" t="inlineStr">
         <is>
-          <t>Brusyliv bourgeois rule of Brusyliv, Radomysl county</t>
+          <t>Брусилівське міщанське правління м-ко Брусилів, Радомисльського повіту</t>
         </is>
       </c>
       <c r="C251" s="27" t="inlineStr">
@@ -8028,7 +8028,7 @@
       </c>
       <c r="B252" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial for Elections to the State Duma of the 2nd convocation Commission of Zhytomyr</t>
+          <t>Волинська губернська у справах про вибори до Державної Думи 2-го скликання комісія м. Житомир</t>
         </is>
       </c>
       <c r="C252" s="27" t="inlineStr">
@@ -8055,7 +8055,7 @@
       </c>
       <c r="B253" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial for Elections to the State Duma of the 3rd convocation Commission of Zhytomyr, Volyn Province</t>
+          <t>Волинська губернська у справах про вибори до Державної Думи 3-го скликання комісія м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C253" s="27" t="inlineStr">
@@ -8082,7 +8082,7 @@
       </c>
       <c r="B254" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial for Elections to the State Duma of the 4th convocation Commission of Zhytomyr</t>
+          <t>Волинська губернська у справах про вибори до Державної Думи 4-го скликання комісія м. Житомир</t>
         </is>
       </c>
       <c r="C254" s="27" t="inlineStr">
@@ -8109,7 +8109,7 @@
       </c>
       <c r="B255" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volynsk district in cases of elections to the State Duma of the 3rd convocation Commission of Novograd-Volynskyi, Volyn Province</t>
+          <t>Новоград-Волинська повітова у справах про вибори до Державної Думи 3-го скликання комісія м. Новоград-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C255" s="27" t="inlineStr">
@@ -8136,7 +8136,7 @@
       </c>
       <c r="B256" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr district in cases of elections to the State Duma of the 2nd convocation Commission of Zhytomyr, Volyn province</t>
+          <t>Житомирська повітова у справах про вибори до Державної Думи 2-го скликання комісія м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C256" s="27" t="inlineStr">
@@ -8163,7 +8163,7 @@
       </c>
       <c r="B257" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr County in cases of elections to the State Duma of the 3rd convocation Commission of Zhytomyr, Volyn Province</t>
+          <t>Житомирська повітова у справах про вибори до Державної Думи 3-го скликання комісія м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C257" s="27" t="inlineStr">
@@ -8190,7 +8190,7 @@
       </c>
       <c r="B258" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr County Committee of Public Health of Zhytomyr, Volyn Province</t>
+          <t>Житомирський повітовий комітет громадського здоров'я м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C258" s="27" t="inlineStr">
@@ -8217,7 +8217,7 @@
       </c>
       <c r="B259" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Valuation Committee of Zhytomyr, Volyn Province</t>
+          <t>Волинський губернський оціночний комітет м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C259" s="27" t="inlineStr">
@@ -8244,7 +8244,7 @@
       </c>
       <c r="B260" s="6" t="inlineStr">
         <is>
-          <t>The second Radomysl county is Radomysl, Kyiv province</t>
+          <t>Друге Радомисльське повітове чиншове присутствіє м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C260" s="27" t="inlineStr">
@@ -8271,7 +8271,7 @@
       </c>
       <c r="B261" s="6" t="inlineStr">
         <is>
-          <t>Radomysl County Staff of Radomysl, Kyiv Province</t>
+          <t>Радомисльський повітовий штабслікар м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C261" s="27" t="inlineStr">
@@ -8298,7 +8298,7 @@
       </c>
       <c r="B262" s="6" t="inlineStr">
         <is>
-          <t>Radomysl county leader of the nobility of Radomysl, Kyiv province</t>
+          <t>Радомисльський повітовий предводитель дворянства м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C262" s="27" t="inlineStr">
@@ -8325,7 +8325,7 @@
       </c>
       <c r="B263" s="6" t="inlineStr">
         <is>
-          <t>Authorized 5th state of Radomysl County</t>
+          <t>Пристав 5-го стану Радомисльського повіту</t>
         </is>
       </c>
       <c r="C263" s="27" t="inlineStr">
@@ -8352,7 +8352,7 @@
       </c>
       <c r="B264" s="6" t="inlineStr">
         <is>
-          <t>Radomysl County Zemsky Administration of Radomysl, Kyiv Province</t>
+          <t>Радомисльська повітова земська управа м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C264" s="27" t="inlineStr">
@@ -8379,7 +8379,7 @@
       </c>
       <c r="B265" s="6" t="inlineStr">
         <is>
-          <t>Volyn Upper Zemsky Court of Zhytomyr, Volyn Province</t>
+          <t>Волинський верхній земський суд м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C265" s="27" t="inlineStr">
@@ -8406,7 +8406,7 @@
       </c>
       <c r="B266" s="6" t="inlineStr">
         <is>
-          <t>Radomysl noble care of Radomysl, Kyiv province</t>
+          <t>Радомисльська дворянська опіка м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C266" s="27" t="inlineStr">
@@ -8433,7 +8433,7 @@
       </c>
       <c r="B267" s="6" t="inlineStr">
         <is>
-          <t>The judicial investigator of the 3rd section of Radomysl County</t>
+          <t>Судовий слідчий 3-ої дільниці Радомисльського повіту</t>
         </is>
       </c>
       <c r="C267" s="27" t="inlineStr">
@@ -8460,7 +8460,7 @@
       </c>
       <c r="B268" s="6" t="inlineStr">
         <is>
-          <t>Radomysl County Treasury of Radomysl, Kyiv Province</t>
+          <t>Радомисльське повітове казначейство м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C268" s="27" t="inlineStr">
@@ -8487,7 +8487,7 @@
       </c>
       <c r="B269" s="6" t="inlineStr">
         <is>
-          <t>Radomysl Zemsky Court of Radomysl, Kyiv Province</t>
+          <t>Радомисльський земський суд м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C269" s="27" t="inlineStr">
@@ -8514,7 +8514,7 @@
       </c>
       <c r="B270" s="6" t="inlineStr">
         <is>
-          <t>Radomysl County Police Department of Radomysl, Kyiv Province</t>
+          <t>Радомисльське повітове поліцейське управління м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C270" s="27" t="inlineStr">
@@ -8541,7 +8541,7 @@
       </c>
       <c r="B271" s="6" t="inlineStr">
         <is>
-          <t>Radomysl Podomen Court of Radomysl, Kyiv Province</t>
+          <t>Радомисльський підкоморський суд м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C271" s="27" t="inlineStr">
@@ -8568,7 +8568,7 @@
       </c>
       <c r="B272" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr Postage and Telegraph Branch of the IV Department of Transportation of Mail by Railway Zhytomyr, Volyn Province</t>
+          <t>Житомирське пошово-телеграфне відділення ІV відділу перевезення пошти залізницею м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C272" s="27" t="inlineStr">
@@ -8595,7 +8595,7 @@
       </c>
       <c r="B273" s="6" t="inlineStr">
         <is>
-          <t>People's Postal and Telegraph Branch of the Kyiv Postal and Telegraph District</t>
+          <t>Народицьке поштово-телеграфне відділення Київської поштово-телеграфної округи м-ко Народичі, Овруцького повіту</t>
         </is>
       </c>
       <c r="C273" s="27" t="inlineStr">
@@ -8622,7 +8622,7 @@
       </c>
       <c r="B274" s="6" t="inlineStr">
         <is>
-          <t>Kmitivsk Postal and Telegraph Branch of the Kiev Postal and Telegraph District Kmitiv, Zhytomyr County</t>
+          <t>Кмитівське поштово-телеграфне відділення Київського поштово-телеграфного округу с. Кмитів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C274" s="27" t="inlineStr">
@@ -8649,7 +8649,7 @@
       </c>
       <c r="B275" s="6" t="inlineStr">
         <is>
-          <t>Pulin Postal and Telegraph Office of the Kiev Postal and Telegraph District</t>
+          <t>Пулинське поштово-телеграфне відділення Київського поштово-телеграфного округу м-ко Пулини, Житомирського повіту</t>
         </is>
       </c>
       <c r="C275" s="27" t="inlineStr">
@@ -8676,7 +8676,7 @@
       </c>
       <c r="B276" s="6" t="inlineStr">
         <is>
-          <t>Ushomir postal and telegraph office</t>
+          <t>Ушомирська поштово-телеграфна контора м-ко Ушомир, Житомирського повіту</t>
         </is>
       </c>
       <c r="C276" s="27" t="inlineStr">
@@ -8703,7 +8703,7 @@
       </c>
       <c r="B277" s="6" t="inlineStr">
         <is>
-          <t>Yanushpil Postal and Telegraph Branch of Yanushpil, Zhytomyr County</t>
+          <t>Янушпільське поштово-телеграфне відділення м-ко Янушпіль, Житомирського повіту</t>
         </is>
       </c>
       <c r="C277" s="27" t="inlineStr">
@@ -8730,7 +8730,7 @@
       </c>
       <c r="B278" s="6" t="inlineStr">
         <is>
-          <t>Martynovichi District Government of the village. Martynovichi, Radomysl county</t>
+          <t>Мартиновицьке волосне правління с. Мартиновичі, Радомисльського повіту</t>
         </is>
       </c>
       <c r="C278" s="27" t="inlineStr">
@@ -8757,7 +8757,7 @@
       </c>
       <c r="B279" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volynsky Orphan Court of Nov.-Volynsky, Volyn province</t>
+          <t>Новоград-Волинський сирітський суд м. Нов.-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C279" s="27" t="inlineStr">
@@ -8784,7 +8784,7 @@
       </c>
       <c r="B280" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Prison Inspectorate of Zhytomyr, Volyn Province</t>
+          <t>Волинська губернська тюремна інспекція м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C280" s="27" t="inlineStr">
@@ -8811,7 +8811,7 @@
       </c>
       <c r="B281" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volyn noble care of Novograd-Volynsky, Volyn province</t>
+          <t>Новоград-Волинська дворянська опіка м. Новоград-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C281" s="27" t="inlineStr">
@@ -8838,7 +8838,7 @@
       </c>
       <c r="B282" s="6" t="inlineStr">
         <is>
-          <t>Vorssovsky District Board of the village. Vorsovka, Radomysl County</t>
+          <t>Ворсівське волосне правління с. Ворсівка, Радомисльського повіту</t>
         </is>
       </c>
       <c r="C282" s="27" t="inlineStr">
@@ -8865,7 +8865,7 @@
       </c>
       <c r="B283" s="6" t="inlineStr">
         <is>
-          <t>Novograd-Volynskyi county leader of the nobility of Novograd-Volynskyi</t>
+          <t>Новоград-Волинський повітовий предводитель дворянства м. Новоград-Волинський</t>
         </is>
       </c>
       <c r="C283" s="27" t="inlineStr">
@@ -8892,7 +8892,7 @@
       </c>
       <c r="B284" s="6" t="inlineStr">
         <is>
-          <t>The Medical Mediator of the 1st District of Volyn County of Novograd-Volynsky, Volyn Province</t>
+          <t>Мировий посередник 1-ої дільниці Волинського повіту м. Новоград-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C284" s="27" t="inlineStr">
@@ -8919,7 +8919,7 @@
       </c>
       <c r="B285" s="6" t="inlineStr">
         <is>
-          <t>Khutorinsky Postal and Telegraph Branch of Krasnopil, Zhytomyr County</t>
+          <t>Хуторинське поштово-телеграфне відділення м-ко Краснопіль, Житомирського повіту</t>
         </is>
       </c>
       <c r="C285" s="27" t="inlineStr">
@@ -8946,7 +8946,7 @@
       </c>
       <c r="B286" s="6" t="inlineStr">
         <is>
-          <t>The sub-inspector of the 1st section of the Radomysl district, Radomysl, Kyiv province</t>
+          <t>Податний інспектор 1-ої дільниці Радомисльського повіту, м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C286" s="27" t="inlineStr">
@@ -8973,7 +8973,7 @@
       </c>
       <c r="B287" s="6" t="inlineStr">
         <is>
-          <t>Malinsky District Board of Mal Malin, Radomysl County, Kyiv Province</t>
+          <t>Малинське волосне правління м-ко Малин, Радомисльського повіту, Київської губернії</t>
         </is>
       </c>
       <c r="C287" s="27" t="inlineStr">
@@ -9000,7 +9000,7 @@
       </c>
       <c r="B288" s="6" t="inlineStr">
         <is>
-          <t>Potiivskaya reign of the village. Potiivka, Radomysl county, Kyiv province</t>
+          <t>Потіївське волосне правління с. Потіївка, Радомисльського повіту, Київської губернії</t>
         </is>
       </c>
       <c r="C288" s="27" t="inlineStr">
@@ -9027,7 +9027,7 @@
       </c>
       <c r="B289" s="6" t="inlineStr">
         <is>
-          <t>Office of Radomysl County Military Chief of Radomysl, Kyiv Province</t>
+          <t>Управління Радомисльського повітового військового начальника м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C289" s="27" t="inlineStr">
@@ -9054,7 +9054,7 @@
       </c>
       <c r="B290" s="6" t="inlineStr">
         <is>
-          <t>Korostyshiv bourgeois administration of Korostyshiv, Radomysl county</t>
+          <t>Коростишівська міщанська управа м-ко Коростишів, Радомисльського повіту</t>
         </is>
       </c>
       <c r="C290" s="27" t="inlineStr">
@@ -9081,7 +9081,7 @@
       </c>
       <c r="B291" s="6" t="inlineStr">
         <is>
-          <t>Korostyshiv District Board of Korostyshiv, Radomysl County</t>
+          <t>Коростишівське волосне правління м-ко Коростишів, Радомисльського повіту</t>
         </is>
       </c>
       <c r="C291" s="27" t="inlineStr">
@@ -9108,7 +9108,7 @@
       </c>
       <c r="B292" s="6" t="inlineStr">
         <is>
-          <t>Nanovsky District Board of the village. Nanivka, Radomysl County</t>
+          <t>Нянівське волосне правління с. Нянівка, Радомисльського повіту</t>
         </is>
       </c>
       <c r="C292" s="27" t="inlineStr">
@@ -9135,7 +9135,7 @@
       </c>
       <c r="B293" s="6" t="inlineStr">
         <is>
-          <t>Shershnovsky District Board of the village. Hornets, Radomysl County</t>
+          <t>Шершнівське волосне правління с. Шершні, Радомисльського повіту</t>
         </is>
       </c>
       <c r="C293" s="27" t="inlineStr">
@@ -9162,7 +9162,7 @@
       </c>
       <c r="B294" s="6" t="inlineStr">
         <is>
-          <t>Volyn Enlightenment Society Zhytomyr, Volyn Province</t>
+          <t>Товариство «Волинська просвіта» м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C294" s="27" t="inlineStr">
@@ -9189,7 +9189,7 @@
       </c>
       <c r="B295" s="6" t="inlineStr">
         <is>
-          <t>Directorate of Zhytomyr Railway Zhytomyr, Volyn Province</t>
+          <t>Управління Житомирської залізниці м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C295" s="27" t="inlineStr">
@@ -9216,7 +9216,7 @@
       </c>
       <c r="B296" s="6" t="inlineStr">
         <is>
-          <t>Department of Novograd-Volyn County Military Chief of Novograd-Volynskyi, Volyn Province</t>
+          <t>Управління Новоград-Волинського повітового військового начальника м. Новоград-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C296" s="27" t="inlineStr">
@@ -9243,7 +9243,7 @@
       </c>
       <c r="B297" s="6" t="inlineStr">
         <is>
-          <t>Ivankovsky bourgeois board of Ivankiv, Radomysl County</t>
+          <t>Іванківське міщанське правління м-ко Іванків, Радомисльського повіту</t>
         </is>
       </c>
       <c r="C297" s="27" t="inlineStr">
@@ -9270,7 +9270,7 @@
       </c>
       <c r="B298" s="6" t="inlineStr">
         <is>
-          <t>Volyn Provincial Food Commission of Zhytomyr, Volyn Province</t>
+          <t>Волинська губернська продовольча комісія м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C298" s="27" t="inlineStr">
@@ -9297,7 +9297,7 @@
       </c>
       <c r="B299" s="6" t="inlineStr">
         <is>
-          <t>Malinsky District Court Mal Malin, Radomysl County</t>
+          <t>Малинський волосний суд м-ко Малин, Радомисльського повіту</t>
         </is>
       </c>
       <c r="C299" s="27" t="inlineStr">
@@ -9324,7 +9324,7 @@
       </c>
       <c r="B300" s="6" t="inlineStr">
         <is>
-          <t>Radomysl Bar of Radomysl, Kyiv province</t>
+          <t>Радомисльська міщанська управа м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C300" s="27" t="inlineStr">
@@ -9351,7 +9351,7 @@
       </c>
       <c r="B301" s="6" t="inlineStr">
         <is>
-          <t>Radomysl County Committee on Affairs on Presentation of the Radomysl, Kyiv Province</t>
+          <t>Радомисльський повітовий комітет у справах по предявленню відстрочок військовозобов'язаними м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C301" s="27" t="inlineStr">
@@ -9378,7 +9378,7 @@
       </c>
       <c r="B302" s="6" t="inlineStr">
         <is>
-          <t>Malinskaya bourgeois management</t>
+          <t>Малинська міщанська управа м-ко Малин, Радомисльського повіту</t>
         </is>
       </c>
       <c r="C302" s="27" t="inlineStr">
@@ -9405,7 +9405,7 @@
       </c>
       <c r="B303" s="6" t="inlineStr">
         <is>
-          <t>Chudniv Roman Catholic Church of Chudnov, Zhytomyr County</t>
+          <t>Чуднівський римо-католицький костьол м-ко Чуднів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C303" s="27" t="inlineStr">
@@ -9432,7 +9432,7 @@
       </c>
       <c r="B304" s="6" t="inlineStr">
         <is>
-          <t>Chudnivsky District Government of M. Chudnov, Zhytomyr County</t>
+          <t>Чуднівське волосне правління м-ко Чуднів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C304" s="27" t="inlineStr">
@@ -9459,7 +9459,7 @@
       </c>
       <c r="B305" s="6" t="inlineStr">
         <is>
-          <t>Chudnivsky bourgeois administration of miracle, Zhytomyr county</t>
+          <t>Чуднівська міщанська управа м-ко Чуднів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C305" s="27" t="inlineStr">
@@ -9486,7 +9486,7 @@
       </c>
       <c r="B306" s="6" t="inlineStr">
         <is>
-          <t>Congress of Mary Judges of Novograd-Volyn Judicial-Mirovy District of Novograd-Volynsky, Volyn Province</t>
+          <t>З'їзд мирових суддів Новоград-Волинського судово-мирового округу м. Новоград-Волинський, Волинської губернії</t>
         </is>
       </c>
       <c r="C306" s="27" t="inlineStr">
@@ -9513,7 +9513,7 @@
       </c>
       <c r="B307" s="6" t="inlineStr">
         <is>
-          <t>Andrushevsky People's School of Andrushivka, Zhytomyr County</t>
+          <t>Андрушівське народне училище м-ко Андрушівка, Житомирського повіту</t>
         </is>
       </c>
       <c r="C307" s="27" t="inlineStr">
@@ -9540,7 +9540,7 @@
       </c>
       <c r="B308" s="6" t="inlineStr">
         <is>
-          <t>Chudnivsky Postal and Telegraph Office</t>
+          <t>Чуднівська поштово-телеграфна контора м-ко Чуднів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C308" s="27" t="inlineStr">
@@ -9567,7 +9567,7 @@
       </c>
       <c r="B309" s="6" t="inlineStr">
         <is>
-          <t>Korovinets Sugar Factory Large coonds. Zhytomyr County</t>
+          <t>Коровинецький цукровий завод с. Великі Коовинці. Житомирського повіту</t>
         </is>
       </c>
       <c r="C309" s="27" t="inlineStr">
@@ -9594,7 +9594,7 @@
       </c>
       <c r="B310" s="6" t="inlineStr">
         <is>
-          <t>Volyn diocesan care over the poor spiritual rank of Zhytomyr, Volyn province</t>
+          <t>Волинська єпархіальна опіка над бідними духовного звання м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C310" s="27" t="inlineStr">
@@ -9621,7 +9621,7 @@
       </c>
       <c r="B311" s="6" t="inlineStr">
         <is>
-          <t>Radomysl spiritual rule of Radomysl, Kyiv province</t>
+          <t>Радомисльське духовне правління м. Радомисль, Київської губернії</t>
         </is>
       </c>
       <c r="C311" s="27" t="inlineStr">
@@ -9648,7 +9648,7 @@
       </c>
       <c r="B312" s="6" t="inlineStr">
         <is>
-          <t>St. Ivan's Church of the Theologian Troshch, Krasnopil parish, Zhytomyr county</t>
+          <t>Церква Св. Іванна Богослова с. Троща, Краснопільської волості, Житомирського повіту</t>
         </is>
       </c>
       <c r="C312" s="27" t="inlineStr">
@@ -9675,7 +9675,7 @@
       </c>
       <c r="B313" s="6" t="inlineStr">
         <is>
-          <t>St. Michael's Church Turchynivka Pykkovskaya Volost, Zhytomyr County</t>
+          <t>Св. Михайлівська церква с. Турчинівка П'ятківської волості, Житомирського повіту</t>
         </is>
       </c>
       <c r="C313" s="27" t="inlineStr">
@@ -9702,7 +9702,7 @@
       </c>
       <c r="B314" s="6" t="inlineStr">
         <is>
-          <t>St. Dimitriivsky Church Burkivtsi, Krasnopil parish, Zhytomyr county</t>
+          <t>Св. Димитріївська церква с. Бурківці, Краснопільської волості, Житомирського повіту</t>
         </is>
       </c>
       <c r="C314" s="27" t="inlineStr">
@@ -9729,7 +9729,7 @@
       </c>
       <c r="B315" s="6" t="inlineStr">
         <is>
-          <t>Church of the Kazan Icon of the Mother of God p. Grandmothers, Pykkovskaya parish, Zhytomyr county</t>
+          <t>Церква Казанської ікони Божої матері с. Бабушки, П'ятківської волості, Житомирського повіту</t>
         </is>
       </c>
       <c r="C315" s="27" t="inlineStr">
@@ -9756,7 +9756,7 @@
       </c>
       <c r="B316" s="6" t="inlineStr">
         <is>
-          <t>St. Michael's Church Motruns, Krasnopil parish, Zhytomyr county</t>
+          <t>Св. Михайлівська церква с. Мотрунки, Краснопільської волості, Житомирського повіту</t>
         </is>
       </c>
       <c r="C316" s="27" t="inlineStr">
@@ -9783,7 +9783,7 @@
       </c>
       <c r="B317" s="6" t="inlineStr">
         <is>
-          <t>St. Trinity Church of Chudnov, Zhytomyr County</t>
+          <t>Св. Троїцька церква м-ко Чуднів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C317" s="27" t="inlineStr">
@@ -9810,7 +9810,7 @@
       </c>
       <c r="B318" s="6" t="inlineStr">
         <is>
-          <t>Cross Church of the village Golivka, Januschpil parish, Zhytomyr county</t>
+          <t>Хрестовоздвиженська церква с. Голіївка, Янушпільської волості, Житомирського повіту</t>
         </is>
       </c>
       <c r="C318" s="27" t="inlineStr">
@@ -9837,7 +9837,7 @@
       </c>
       <c r="B319" s="6" t="inlineStr">
         <is>
-          <t>Cross Church of the village Dadkovtsi, Chudnivskyi parish, Zhytomyr county</t>
+          <t>Хрестовоздвиженська церква с. Дідківці, Чуднівської волості, Житомирського повіту</t>
         </is>
       </c>
       <c r="C319" s="27" t="inlineStr">
@@ -9864,7 +9864,7 @@
       </c>
       <c r="B320" s="6" t="inlineStr">
         <is>
-          <t>Church of the Nativity of the Virgin Mary Nosovka, Krasnopil Vost, Zhytomyr County</t>
+          <t>Церква Різдва Богородиці с. Носівка, Краснопільської волості, Житомирського повіту</t>
         </is>
       </c>
       <c r="C320" s="27" t="inlineStr">
@@ -9891,7 +9891,7 @@
       </c>
       <c r="B321" s="6" t="inlineStr">
         <is>
-          <t>Roman Catholic Church Mr. Krasnopil, Zhytomyr County</t>
+          <t>Римо-католицький костьол м-ка Краснопіль, Житомирського повіту</t>
         </is>
       </c>
       <c r="C321" s="27" t="inlineStr">
@@ -9918,7 +9918,7 @@
       </c>
       <c r="B322" s="6" t="inlineStr">
         <is>
-          <t>Chudnivska Pleasure Mr. Chudnov Zhytomyr County</t>
+          <t>Чуднівське благочиніє м-ко Чуднів Житомирського повіту</t>
         </is>
       </c>
       <c r="C322" s="27" t="inlineStr">
@@ -9945,7 +9945,7 @@
       </c>
       <c r="B323" s="6" t="inlineStr">
         <is>
-          <t>St. Nikolaev Church of the city</t>
+          <t>Св. Миколаївська церква м-ка Червоне, Солотвинської вол., Житомирського повіту</t>
         </is>
       </c>
       <c r="C323" s="27" t="inlineStr">
@@ -9972,7 +9972,7 @@
       </c>
       <c r="B324" s="6" t="inlineStr">
         <is>
-          <t>Cross Church of the city of Red, Solotvinskay</t>
+          <t>Хрестовоздвиженська церква м-ка Червоне, Солотвинської вол., Житомирського повіту</t>
         </is>
       </c>
       <c r="C324" s="27" t="inlineStr">
@@ -9999,7 +9999,7 @@
       </c>
       <c r="B325" s="6" t="inlineStr">
         <is>
-          <t>St. Dimitriivska Church of the city</t>
+          <t>Св. Димитріївська церква м-ка Червоне, Солотвинської вол., Житомирського повіту</t>
         </is>
       </c>
       <c r="C325" s="27" t="inlineStr">
@@ -10026,7 +10026,7 @@
       </c>
       <c r="B326" s="6" t="inlineStr">
         <is>
-          <t>Roman Catholic Church M. Chudnov, Zhytomyr County</t>
+          <t>Римо-католицький костьол м-ка Чуднів, Житомирського повіту</t>
         </is>
       </c>
       <c r="C326" s="27" t="inlineStr">
@@ -10053,7 +10053,7 @@
       </c>
       <c r="B327" s="6" t="inlineStr">
         <is>
-          <t>St. Pokrovskaya Church Horopai, Novochorrtory Vol., Novograd-Volyn County</t>
+          <t>Св. Покровська церква с. Горопаї, Новочорторийської вол., Новоград-Волинського повіту</t>
         </is>
       </c>
       <c r="C327" s="27" t="inlineStr">
@@ -10080,7 +10080,7 @@
       </c>
       <c r="B328" s="6" t="inlineStr">
         <is>
-          <t>St. Vasyliv Church Gizivshchyna, Derevitsa Vol., Novograd-Volyn County</t>
+          <t>Св. Василівська церква с. Гізівщина, Деревицької вол., Новоград-Волинського повіту</t>
         </is>
       </c>
       <c r="C328" s="27" t="inlineStr">
@@ -10107,7 +10107,7 @@
       </c>
       <c r="B329" s="6" t="inlineStr">
         <is>
-          <t>St. Michael's Church of Krasnopil, Krasnopil Vol., Zhytomyr County</t>
+          <t>Св. Михайлівська церква м-ка Краснопіль, Краснопільськї вол., Житомирського повіту</t>
         </is>
       </c>
       <c r="C329" s="27" t="inlineStr">
@@ -10134,7 +10134,7 @@
       </c>
       <c r="B330" s="6" t="inlineStr">
         <is>
-          <t>St. Trinity Church of the village Milk, Krasnopil Vol., Zhytomyr County</t>
+          <t>Св. Троїцька церква с. Молочки, Краснопільської вол., Житомирського повіту</t>
         </is>
       </c>
       <c r="C330" s="27" t="inlineStr">
@@ -10161,7 +10161,7 @@
       </c>
       <c r="B331" s="6" t="inlineStr">
         <is>
-          <t>Volyn Prison Patronatics in Zhytomyr, Volyn Province</t>
+          <t>Волинський тюремний патронат м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C331" s="27" t="inlineStr">
@@ -10188,7 +10188,7 @@
       </c>
       <c r="B332" s="6" t="inlineStr">
         <is>
-          <t>Provincial inspector of police guard of Zhytomyr, Volyn province</t>
+          <t>Губернський інспектор поліцейської варти м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C332" s="27" t="inlineStr">
@@ -10215,7 +10215,7 @@
       </c>
       <c r="B333" s="6" t="inlineStr">
         <is>
-          <t>Alexander Kututov. Volyn Governor.</t>
+          <t>Кутайсов Олександр Павлович. Волинський губернатор.</t>
         </is>
       </c>
       <c r="C333" s="27" t="inlineStr">
@@ -10242,7 +10242,7 @@
       </c>
       <c r="B334" s="6" t="inlineStr">
         <is>
-          <t>Zhytomyr provincial prison in Zhytomyr, Volyn province</t>
+          <t>Житомирська губернська тюрма м. Житомир, Волинської губернії</t>
         </is>
       </c>
       <c r="C334" s="27" t="inlineStr">
@@ -10269,7 +10269,7 @@
       </c>
       <c r="B335" s="6" t="inlineStr">
         <is>
-          <t>Makhnovsky County Court of Bratslav governorship of the Kiev province. Berdychiv County Court of Kyiv province</t>
+          <t>Махнівський повітовий суд Брацлавського намісництва Київської губернії. Бердичівський повітовий суд Київської губернії</t>
         </is>
       </c>
       <c r="C335" s="27" t="inlineStr">
@@ -10296,7 +10296,7 @@
       </c>
       <c r="B336" s="6" t="inlineStr">
         <is>
-          <t>Berdichevsky County in Chinch Affairs is Berdychiv. Kiev province</t>
+          <t>Бердичівське повітове у чиншових справах присутствіє м. Бердичів. Київської губернії</t>
         </is>
       </c>
       <c r="C336" s="27" t="inlineStr">
@@ -10323,7 +10323,7 @@
       </c>
       <c r="B337" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv Commercial School of Berdychiv, Kyiv Province</t>
+          <t>Бердичівське комерційне училище м. Бердичів, Київської губернії</t>
         </is>
       </c>
       <c r="C337" s="27" t="inlineStr">
@@ -10350,7 +10350,7 @@
       </c>
       <c r="B338" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv noble care of Berdychiv, Kyiv province</t>
+          <t>Бердичівська дворянська опіка м. Бердичів, Київської губернії</t>
         </is>
       </c>
       <c r="C338" s="27" t="inlineStr">
@@ -10377,7 +10377,7 @@
       </c>
       <c r="B339" s="6" t="inlineStr">
         <is>
-          <t>Berdichevsky County Agemir of Berdychiv, Kyiv Province</t>
+          <t>Бердичівський повітовий землемір м. Бердичів, Київської губернії</t>
         </is>
       </c>
       <c r="C339" s="27" t="inlineStr">
@@ -10404,7 +10404,7 @@
       </c>
       <c r="B340" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv City Magistrate of Berdychiv, Kyiv province</t>
+          <t>Бердичівський городовий магістрат м. Бердичів, Київської губернії</t>
         </is>
       </c>
       <c r="C340" s="27" t="inlineStr">
@@ -10431,7 +10431,7 @@
       </c>
       <c r="B341" s="6" t="inlineStr">
         <is>
-          <t>The Kupchikha Store Gorbunova AA</t>
+          <t>Магазин купчихи Горбунової А. А.</t>
         </is>
       </c>
       <c r="C341" s="27" t="inlineStr">
@@ -10458,7 +10458,7 @@
       </c>
       <c r="B342" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv district in cases of elections to the 2nd State Duma Commission of Berdychiv Kyiv province</t>
+          <t>Бердичівська повітова у справах про вибори до 2-ої Державної Думи комісія м. Бердичів Київської губернії</t>
         </is>
       </c>
       <c r="C342" s="27" t="inlineStr">
@@ -10485,7 +10485,7 @@
       </c>
       <c r="B343" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv district in cases of elections to the 1st State Duma Commission of Berdychiv, Kyiv province</t>
+          <t>Бердичівська повітова у справах про вибори до 1-ої Державної Думи комісія м. Бердичів, Київської губернії</t>
         </is>
       </c>
       <c r="C343" s="27" t="inlineStr">
@@ -10512,7 +10512,7 @@
       </c>
       <c r="B344" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv district in cases of elections to the 4th State Duma Commission of Berdychiv, Kyiv province</t>
+          <t>Бердичівська повітова у справах про вибори до 4-ої Державної Думи комісія м. Бердичів, Київської губернії</t>
         </is>
       </c>
       <c r="C344" s="27" t="inlineStr">
@@ -10539,7 +10539,7 @@
       </c>
       <c r="B345" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv district in cases of elections to the 3rd State Duma Commission of Berdychiv, Kyiv province</t>
+          <t>Бердичівська повітова у справах про вибори до 3-ої Державної Думи комісія м. Бердичів, Київської губернії</t>
         </is>
       </c>
       <c r="C345" s="27" t="inlineStr">
@@ -10566,7 +10566,7 @@
       </c>
       <c r="B346" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv district in cases of elections to the State Duma and the State Council Commission of Berdychiv, Kyiv province</t>
+          <t>Бердичівська повітова у справах про вибори до Державної Думи та Державної Ради комісія м. Бердичів, Київської губернії</t>
         </is>
       </c>
       <c r="C346" s="27" t="inlineStr">
@@ -10593,7 +10593,7 @@
       </c>
       <c r="B347" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv Cathedral Assumption Church of Berdychiv, Kyiv province</t>
+          <t>Бердичівська соборна Успенська церква м. Бердичів, Київської губернії</t>
         </is>
       </c>
       <c r="C347" s="27" t="inlineStr">
@@ -10620,7 +10620,7 @@
       </c>
       <c r="B348" s="6" t="inlineStr">
         <is>
-          <t>Belilovsky District Revolution of Mr Belilovka, Berdychiv County</t>
+          <t>Білилівське волосне правління м-ко Білилівка, Бердичівського повіту</t>
         </is>
       </c>
       <c r="C348" s="27" t="inlineStr">
@@ -10647,7 +10647,7 @@
       </c>
       <c r="B349" s="6" t="inlineStr">
         <is>
-          <t>Bystritsky district rule of the village. Bystryk, Berdychiv county</t>
+          <t>Бистрицьке волосне правління с. Бистрик, Бердичівського повіту</t>
         </is>
       </c>
       <c r="C349" s="27" t="inlineStr">
@@ -10674,7 +10674,7 @@
       </c>
       <c r="B350" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv branch of the Russo-French Commercial Bank of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівське відділення російсько-французького комерційного Банку м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C350" s="27" t="inlineStr">
@@ -10701,7 +10701,7 @@
       </c>
       <c r="B351" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv Commercial and Slavic Court of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівський торгово-словесний суд м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C351" s="27" t="inlineStr">
@@ -10728,7 +10728,7 @@
       </c>
       <c r="B352" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv County Zemsky Administration of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівська повітова земська управа м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C352" s="27" t="inlineStr">
@@ -10755,7 +10755,7 @@
       </c>
       <c r="B353" s="6" t="inlineStr">
         <is>
-          <t>Belilovsky village administration of the village. Bilylivka, Berdichevsky str.</t>
+          <t>Білилівське сільське управління с. Білилівка, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C353" s="27" t="inlineStr">
@@ -10782,7 +10782,7 @@
       </c>
       <c r="B354" s="6" t="inlineStr">
         <is>
-          <t>Shirma District Board of Mr. Shirmivka, Berdychiv Piv.</t>
+          <t>Ширмівське волосне правління м-ко Ширмівка, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C354" s="27" t="inlineStr">
@@ -10809,7 +10809,7 @@
       </c>
       <c r="B355" s="6" t="inlineStr">
         <is>
-          <t>Belgorod District Board of Belgorodka, Berdichevsky Plo.</t>
+          <t>Білогородське волосне правління м-ко Білогородка, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C355" s="27" t="inlineStr">
@@ -10836,7 +10836,7 @@
       </c>
       <c r="B356" s="6" t="inlineStr">
         <is>
-          <t>Office of the Berdychiv County Military Chief of Berdychiv, Kiev Lips.</t>
+          <t>Управління Бердичівського повітового військового начальника м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C356" s="27" t="inlineStr">
@@ -10863,7 +10863,7 @@
       </c>
       <c r="B357" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv district police of Berdychiv, Kiev lips.</t>
+          <t>Бердичівська повітова поліція м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C357" s="27" t="inlineStr">
@@ -10890,7 +10890,7 @@
       </c>
       <c r="B358" s="6" t="inlineStr">
         <is>
-          <t>The 3rd state of Berdychiv county</t>
+          <t>Пристав 3-го стану Бердичівського повіту</t>
         </is>
       </c>
       <c r="C358" s="27" t="inlineStr">
@@ -10917,7 +10917,7 @@
       </c>
       <c r="B359" s="6" t="inlineStr">
         <is>
-          <t>Belilov Postal and Telegraph Office of the Kiev Postal and Telegraph District of Bilylivka, Berdychiv County</t>
+          <t>Білилівська поштово-телеграфна контора Київської поштово-телеграфної округи м. Білилівка, Бердичівського повіту</t>
         </is>
       </c>
       <c r="C359" s="27" t="inlineStr">
@@ -10944,7 +10944,7 @@
       </c>
       <c r="B360" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv Police Department of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівське поліцейське управління м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C360" s="27" t="inlineStr">
@@ -10971,7 +10971,7 @@
       </c>
       <c r="B361" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv City Police of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівська міська поліція м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C361" s="27" t="inlineStr">
@@ -10998,7 +10998,7 @@
       </c>
       <c r="B362" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv Postal and Telegraph Office of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівська поштово-телеграфна контора м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C362" s="27" t="inlineStr">
@@ -11025,7 +11025,7 @@
       </c>
       <c r="B363" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv county leader of the nobility of Berdychiv, Kiev lips.</t>
+          <t>Бердичівський повітовий предводитель дворянства м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C363" s="27" t="inlineStr"/>
@@ -11048,7 +11048,7 @@
       </c>
       <c r="B364" s="6" t="inlineStr">
         <is>
-          <t>The Medical Medical 2nd Station of Berdychivsky St.</t>
+          <t>Мировий посередний 2-ої дільниці Бердичівського пов.</t>
         </is>
       </c>
       <c r="C364" s="27" t="inlineStr">
@@ -11075,7 +11075,7 @@
       </c>
       <c r="B365" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv Tylova Evacuation Commission of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівська тилова евакуаційна комісія м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C365" s="27" t="inlineStr">
@@ -11102,7 +11102,7 @@
       </c>
       <c r="B366" s="6" t="inlineStr">
         <is>
-          <t>2nd Berdychiv district layout on an industrial tax is presence of Berdychiv, Kiev lips.</t>
+          <t>2-ге Бердичівське повітове розкладкове по промисловому податку присутствіє м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C366" s="27" t="inlineStr">
@@ -11129,7 +11129,7 @@
       </c>
       <c r="B367" s="6" t="inlineStr">
         <is>
-          <t>Ogiyevsky District Board of the village. Ogiivka, Berdychivskyi, Kyiv Lips.</t>
+          <t>Огіївське волосне правління с. Огіївка, Бердичівського пов., Київської губ.</t>
         </is>
       </c>
       <c r="C367" s="27" t="inlineStr">
@@ -11156,7 +11156,7 @@
       </c>
       <c r="B368" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv Leather Plant of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівський шкіряний завод м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C368" s="27" t="inlineStr">
@@ -11183,7 +11183,7 @@
       </c>
       <c r="B369" s="6" t="inlineStr">
         <is>
-          <t>Society of Berdychiv Sugar-Buryak and Refine Plants of Berdychiv, Kiev Lips.</t>
+          <t>Товариство Бердичівського цукрово-бурякового та рафінадного заводів м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C369" s="27" t="inlineStr">
@@ -11210,7 +11210,7 @@
       </c>
       <c r="B370" s="6" t="inlineStr">
         <is>
-          <t>St. Pokrovskaya Church Bystryk, Berdichevsky str.</t>
+          <t>Св. Покровська церква с. Бистрик, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C370" s="27" t="inlineStr">
@@ -11237,7 +11237,7 @@
       </c>
       <c r="B371" s="6" t="inlineStr">
         <is>
-          <t>St. Trinity Church of Berdychiv, Kiev Lips.</t>
+          <t>Св. Троїцька церква м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C371" s="27" t="inlineStr">
@@ -11264,7 +11264,7 @@
       </c>
       <c r="B372" s="6" t="inlineStr">
         <is>
-          <t>Jewish religious community of mi-ka, Skvyrian district.</t>
+          <t>Єврейська релігійна громада м-ка Вчорайше, Сквирького пов.</t>
         </is>
       </c>
       <c r="C372" s="27" t="inlineStr">
@@ -11291,7 +11291,7 @@
       </c>
       <c r="B373" s="6" t="inlineStr">
         <is>
-          <t>Church of the Nativity of the Virgin Mary of Yanushpil, Zhytomyr</t>
+          <t>Церква Різдва Богородиці м-ка Янушпіль, Житомирського пов.</t>
         </is>
       </c>
       <c r="C373" s="27" t="inlineStr">
@@ -11318,7 +11318,7 @@
       </c>
       <c r="B374" s="6" t="inlineStr">
         <is>
-          <t>Roman Catholic Parish Church M-ka Ruzhin, Skvyr County</t>
+          <t>Римо-католицький парафіяльний костьол м-ка Ружин, Сквирського повіту</t>
         </is>
       </c>
       <c r="C374" s="27" t="inlineStr">
@@ -11345,7 +11345,7 @@
       </c>
       <c r="B375" s="6" t="inlineStr">
         <is>
-          <t>Roman Catholic Parish Church M-ka Lubar. Novograd-Volynskyi floor.</t>
+          <t>Римо-католицький парафіяльний костьол м-ка Любар. Новоград-Волинського пов.</t>
         </is>
       </c>
       <c r="C375" s="27" t="inlineStr">
@@ -11372,7 +11372,7 @@
       </c>
       <c r="B376" s="6" t="inlineStr">
         <is>
-          <t>St. Dimitrovskaya Church Chornoudka Berdichevsky str.</t>
+          <t>Св. Димитрівська церква с. Чорнорудка Бердичівського пов.</t>
         </is>
       </c>
       <c r="C376" s="27" t="inlineStr">
@@ -11399,7 +11399,7 @@
       </c>
       <c r="B377" s="6" t="inlineStr">
         <is>
-          <t>St. George's Church of Bilylivka, Berdichevsky str.</t>
+          <t>Св. Георгіївська  церква м-ка Білилівка, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C377" s="27" t="inlineStr">
@@ -11426,7 +11426,7 @@
       </c>
       <c r="B378" s="6" t="inlineStr">
         <is>
-          <t>St. Trinity Church of Bilylivka, Berdichevsky St.</t>
+          <t>Св. Троїцька церква м-ка Білилівка, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C378" s="27" t="inlineStr">
@@ -11453,7 +11453,7 @@
       </c>
       <c r="B379" s="6" t="inlineStr">
         <is>
-          <t>St. Nikolaev Church Khalaimhorodok, Berdychivsky district.</t>
+          <t>Св. Миколаївська церква с. Халаїмгородок, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C379" s="27" t="inlineStr">
@@ -11480,7 +11480,7 @@
       </c>
       <c r="B380" s="6" t="inlineStr">
         <is>
-          <t>St. Nikolaev Church Singayevka, Berdychiv district.</t>
+          <t>Св. Миколаївська церква с. Сингаївка, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C380" s="27" t="inlineStr">
@@ -11507,7 +11507,7 @@
       </c>
       <c r="B381" s="6" t="inlineStr">
         <is>
-          <t>The Church of St. John the Theologian Zhurbintsi, Makhnovsky district.</t>
+          <t>Церква Св. Іоанна Богослова с. Журбинці, Махнівського пов.</t>
         </is>
       </c>
       <c r="C381" s="27" t="inlineStr">
@@ -11534,7 +11534,7 @@
       </c>
       <c r="B382" s="6" t="inlineStr">
         <is>
-          <t>St. Pokrovskaya Church Zakutins, Berdichevsky district.</t>
+          <t>Св. Покровська церква с. Закутинці, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C382" s="27" t="inlineStr">
@@ -11561,7 +11561,7 @@
       </c>
       <c r="B383" s="6" t="inlineStr">
         <is>
-          <t>The Church of St. John the Theologian Skraglivka, Berdichevsky district.</t>
+          <t>Церква Св. Іоанна Богослова с. Скраглівка, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C383" s="27" t="inlineStr">
@@ -11588,7 +11588,7 @@
       </c>
       <c r="B384" s="6" t="inlineStr">
         <is>
-          <t>Cross Church of the village Pyatgirka, Berdician floor.</t>
+          <t>Хрестовоздвиженська церква с. П'ятигірка, Бердичіського пов.</t>
         </is>
       </c>
       <c r="C384" s="27" t="inlineStr">
@@ -11615,7 +11615,7 @@
       </c>
       <c r="B385" s="6" t="inlineStr">
         <is>
-          <t>St. Pokrovskaya Church Gadomtsi, Berdychiv district.</t>
+          <t>Св. Покровська церква с. Гадомці, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C385" s="27" t="inlineStr">
@@ -11642,7 +11642,7 @@
       </c>
       <c r="B386" s="6" t="inlineStr">
         <is>
-          <t>Anno-Zachatiev Church Zhinka, Berdichevsky str.</t>
+          <t>Анно-Зачатіївська церква с. Житинці, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C386" s="27" t="inlineStr">
@@ -11669,7 +11669,7 @@
       </c>
       <c r="B387" s="6" t="inlineStr">
         <is>
-          <t>Church of the Nativity of the Virgin Mary Krasivka, Berdichevsky district.</t>
+          <t>Церква Різдва Богородиці с. Красівка, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C387" s="27" t="inlineStr">
@@ -11696,7 +11696,7 @@
       </c>
       <c r="B388" s="6" t="inlineStr">
         <is>
-          <t>St. Trinity Church of Krasnopil, Zhytomyr Piv., Vol. lips.</t>
+          <t>Св. Троїцька церква м-ка Краснопіль, Житомирського пов., Вол. губ.</t>
         </is>
       </c>
       <c r="C388" s="27" t="inlineStr">
@@ -11723,7 +11723,7 @@
       </c>
       <c r="B389" s="6" t="inlineStr">
         <is>
-          <t>Cross Church of the village Pyatgirka, Berdichevsky str.</t>
+          <t>Хрестовоздвиженська церква с. П'ятигірка, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C389" s="27" t="inlineStr">
@@ -11750,7 +11750,7 @@
       </c>
       <c r="B390" s="6" t="inlineStr">
         <is>
-          <t>St. Assumption Church Nekhvoroshch, Lipovetskyi, Kyiv Lips.</t>
+          <t>Св. Успенська церква с. Нехворощ, Липовецького пов., Київської губ.</t>
         </is>
       </c>
       <c r="C390" s="27" t="inlineStr">
@@ -11777,7 +11777,7 @@
       </c>
       <c r="B391" s="6" t="inlineStr">
         <is>
-          <t>St. Pokrovskaya Church Terekhova, Berdichevsky district.</t>
+          <t>Св. Покровська церква с. Терехова, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C391" s="27" t="inlineStr">
@@ -11804,7 +11804,7 @@
       </c>
       <c r="B392" s="6" t="inlineStr">
         <is>
-          <t>The Puzyretsky District Board of the village. Puzirki, Berdichevsky str.</t>
+          <t>Пузирецьке волосне правління с. Пузирки, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C392" s="27" t="inlineStr">
@@ -11831,7 +11831,7 @@
       </c>
       <c r="B393" s="6" t="inlineStr">
         <is>
-          <t>St. Dimitrovskaya Church Krylovka, Podorazanskaya Vol., Kyiv Lips.</t>
+          <t>Св. Димитрівська церква с. Крилівка, Подоражанської вол., Київської губ.</t>
         </is>
       </c>
       <c r="C393" s="27" t="inlineStr">
@@ -11858,7 +11858,7 @@
       </c>
       <c r="B394" s="6" t="inlineStr">
         <is>
-          <t>Carmelitan Roman Catholic Church Berdychiv, Kiev lips.</t>
+          <t>Кармелітанський римо-католицький костьол с. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C394" s="27" t="inlineStr">
@@ -11885,7 +11885,7 @@
       </c>
       <c r="B395" s="6" t="inlineStr">
         <is>
-          <t>St. Dimitriivsky Church Ivankivtsi, Berdichevsky district.</t>
+          <t>Св. Димитріївська церква с. Іванківці, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C395" s="27" t="inlineStr">
@@ -11912,7 +11912,7 @@
       </c>
       <c r="B396" s="6" t="inlineStr">
         <is>
-          <t>Roman Catholic Parish Church M-ka Scarry, Skvyr County</t>
+          <t>Римо-католицький парафіяльний костьол м-ка Вчорайше, Сквирського повіту</t>
         </is>
       </c>
       <c r="C396" s="27" t="inlineStr">
@@ -11939,7 +11939,7 @@
       </c>
       <c r="B397" s="6" t="inlineStr">
         <is>
-          <t>St. Pokrovskaya Church Galchin, Zhytomyr County</t>
+          <t>Св. Покровська церква с. Гальчин, Житомирського повіту</t>
         </is>
       </c>
       <c r="C397" s="27" t="inlineStr">
@@ -11966,7 +11966,7 @@
       </c>
       <c r="B398" s="6" t="inlineStr">
         <is>
-          <t>St. Michael's Church of M-ka, Skvyrsky district.</t>
+          <t>Св. Михайлівська церква м-ка Вчорайше, Сквирського пов.</t>
         </is>
       </c>
       <c r="C398" s="27" t="inlineStr">
@@ -11993,7 +11993,7 @@
       </c>
       <c r="B399" s="6" t="inlineStr">
         <is>
-          <t>St. Paraskeev Church of the village Big Nizhirka, Berdychiv district.</t>
+          <t>Св. Параскевівська церква с. Великі Низгірці, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C399" s="27" t="inlineStr">
@@ -12020,7 +12020,7 @@
       </c>
       <c r="B400" s="6" t="inlineStr">
         <is>
-          <t>St. Panteleimon Church Korchmyshche, Skvyrsky district.</t>
+          <t>Св. Пантелеймонівська церква с. Корчмище, Сквирського пов.</t>
         </is>
       </c>
       <c r="C400" s="27" t="inlineStr">
@@ -12047,7 +12047,7 @@
       </c>
       <c r="B401" s="6" t="inlineStr">
         <is>
-          <t>S. Michael's Church Yagnatyn, Skvyrsky floor.</t>
+          <t>С. Михайлівська церква с. Ягнятин, Сквирського пов.</t>
         </is>
       </c>
       <c r="C401" s="27" t="inlineStr">
@@ -12074,7 +12074,7 @@
       </c>
       <c r="B402" s="6" t="inlineStr">
         <is>
-          <t>The Society of the Svoynets Sugar Factory</t>
+          <t>Товариство Спичинецького цукрового заводу</t>
         </is>
       </c>
       <c r="C402" s="27" t="inlineStr">
@@ -12101,7 +12101,7 @@
       </c>
       <c r="B403" s="6" t="inlineStr">
         <is>
-          <t>St. Mitrofaniyevsky Church of the village. Minkivtsi Lipovetsky County, Kiev Lips.</t>
+          <t>Св. Митрофаніївська церква с. Миньківці Липовецького повіту, Київської губ.</t>
         </is>
       </c>
       <c r="C403" s="27" t="inlineStr">
@@ -12128,7 +12128,7 @@
       </c>
       <c r="B404" s="6" t="inlineStr">
         <is>
-          <t>Vozdvizhensk Church Mala Chernyavka, Berdichevsky str.</t>
+          <t>Воздвиженська церква с. Мала Чернявка, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C404" s="27" t="inlineStr">
@@ -12155,7 +12155,7 @@
       </c>
       <c r="B405" s="6" t="inlineStr">
         <is>
-          <t>The Church of the Holy Apostle Luke p. Semenivka, Berdichevsky St.</t>
+          <t>Церква Св. Апостола Луки с. Семенівка, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C405" s="27" t="inlineStr">
@@ -12182,7 +12182,7 @@
       </c>
       <c r="B406" s="6" t="inlineStr">
         <is>
-          <t>Church of the Nativity of the Virgin Mary Stones, Skvyrsky floor.</t>
+          <t>Церква Різдва Богородиці с. Камені, Сквирського пов.</t>
         </is>
       </c>
       <c r="C406" s="27" t="inlineStr">
@@ -12209,7 +12209,7 @@
       </c>
       <c r="B407" s="6" t="inlineStr">
         <is>
-          <t>St. Pokrovskaya Church Flat, Skvyrsky floor.</t>
+          <t>Св. Покровська церква с. Плоска, Сквирського пов.</t>
         </is>
       </c>
       <c r="C407" s="27" t="inlineStr">
@@ -12236,7 +12236,7 @@
       </c>
       <c r="B408" s="6" t="inlineStr">
         <is>
-          <t>Church of the Nativity of the Virgin Mary Negvroshch, Zhytomyr district.</t>
+          <t>Церква Різдва Богородиці с. Нехворощ, Житомирського пов.</t>
         </is>
       </c>
       <c r="C408" s="27" t="inlineStr">
@@ -12263,7 +12263,7 @@
       </c>
       <c r="B409" s="6" t="inlineStr">
         <is>
-          <t>The Stetkovetske pious village. Stetkivtsi, Yanushpil Vol., Zhytomyr St.</t>
+          <t>Стетковецьке благочиніє с. Стетківці, Янушпільської вол., Житомирського пов.</t>
         </is>
       </c>
       <c r="C409" s="27" t="inlineStr">
@@ -12290,7 +12290,7 @@
       </c>
       <c r="B410" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv spiritual rule of Berdychiv, Kiev lips.</t>
+          <t>Бердичівське духовне правління м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C410" s="27" t="inlineStr">
@@ -12317,7 +12317,7 @@
       </c>
       <c r="B411" s="6" t="inlineStr">
         <is>
-          <t>St. Trinity Church of the village Slobodyshche, Pykkovskaya Vol., Zhytomyr district.</t>
+          <t>Св. Троїцька церква с. Слободище, П'ятківської вол., Житомирського пов.</t>
         </is>
       </c>
       <c r="C411" s="27" t="inlineStr">
@@ -12344,7 +12344,7 @@
       </c>
       <c r="B412" s="6" t="inlineStr">
         <is>
-          <t>Miracle Church Markushi, Berdichevsky str.</t>
+          <t>Чудо-Михайлівська церква с. Маркуші, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C412" s="27" t="inlineStr">
@@ -12371,7 +12371,7 @@
       </c>
       <c r="B413" s="6" t="inlineStr">
         <is>
-          <t>Roman Catholic Parish Church of St. Barbara Berdychiv, Kiev Lips.</t>
+          <t>Римо-католицький парафіяльний костьол Святої Варвари м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C413" s="27" t="inlineStr">
@@ -12398,7 +12398,7 @@
       </c>
       <c r="B414" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv Boarding Board of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівська міщанська управа м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C414" s="27" t="inlineStr">
@@ -12425,7 +12425,7 @@
       </c>
       <c r="B415" s="6" t="inlineStr">
         <is>
-          <t>The Berdychiv Investigation Commission was founded by the Assumption Church of Berdychiv, Zhytomyr district.</t>
+          <t>Бердичівська слідча комісія заснована Успенською церквою м-ко Бердичів, Житомирського пов.</t>
         </is>
       </c>
       <c r="C415" s="27" t="inlineStr">
@@ -12452,7 +12452,7 @@
       </c>
       <c r="B416" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv district from military service is present in Berdychiv, Kiev lips.</t>
+          <t>Бердичівське повітове з військової повинності присутствіє м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C416" s="27" t="inlineStr">
@@ -12479,7 +12479,7 @@
       </c>
       <c r="B417" s="6" t="inlineStr">
         <is>
-          <t>Belilovsky bourgeois administration of Mr. Bilylivka, Berdychiv district.</t>
+          <t>Білилівська міщанська управа м-ко Білилівка, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C417" s="27" t="inlineStr">
@@ -12506,7 +12506,7 @@
       </c>
       <c r="B418" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv County Zemsky Assembly of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівські повітові земські збори м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C418" s="27" t="inlineStr">
@@ -12533,7 +12533,7 @@
       </c>
       <c r="B419" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv County Treasury of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівське повітове казначейство м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C419" s="27" t="inlineStr">
@@ -12560,7 +12560,7 @@
       </c>
       <c r="B420" s="6" t="inlineStr">
         <is>
-          <t>Judicial Investigator of Berdychiv, Kyiv Lips.</t>
+          <t>Судовий слідчий м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C420" s="27" t="inlineStr">
@@ -12587,7 +12587,7 @@
       </c>
       <c r="B421" s="6" t="inlineStr">
         <is>
-          <t>Belilovskaya loan-savings cash desk of Mr Belilovka, Berdychivskyi.</t>
+          <t>Білилівська волосна позичково-ощадна каса м-ко Білилівка, Бердичівського пов.</t>
         </is>
       </c>
       <c r="C421" s="27" t="inlineStr">
@@ -12614,7 +12614,7 @@
       </c>
       <c r="B422" s="6" t="inlineStr">
         <is>
-          <t>The Medical Mediator of the 1st Station of Berdychivsky St.</t>
+          <t>Мировий посередник 1-ої дільниці Бердичівського пов.</t>
         </is>
       </c>
       <c r="C422" s="27" t="inlineStr">
@@ -12641,7 +12641,7 @@
       </c>
       <c r="B423" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv City Administration of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівська міська управа м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C423" s="27" t="inlineStr">
@@ -12668,7 +12668,7 @@
       </c>
       <c r="B424" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv County Soviet City of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівський повітовий стряпчий м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C424" s="27" t="inlineStr">
@@ -12695,7 +12695,7 @@
       </c>
       <c r="B425" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv-Lipovetsky Congress of Peacemakers of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівсько-Липовецький з'їзд мирових посередників м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C425" s="27" t="inlineStr">
@@ -12722,7 +12722,7 @@
       </c>
       <c r="B426" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv Orphan Court of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівський сирітський суд м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C426" s="27" t="inlineStr">
@@ -12749,7 +12749,7 @@
       </c>
       <c r="B427" s="6" t="inlineStr">
         <is>
-          <t>The 1st state of Berdychiv county</t>
+          <t>Пристав 1-го стану Бердичівського повіту</t>
         </is>
       </c>
       <c r="C427" s="27" t="inlineStr">
@@ -12776,7 +12776,7 @@
       </c>
       <c r="B428" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv City Duma of Berdychiv, Kiev Lips.</t>
+          <t>Бердичівська міська дума м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C428" s="27" t="inlineStr">
@@ -12803,7 +12803,7 @@
       </c>
       <c r="B429" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv notary MD Klinkovstin, Berdychiv, Kiev Lips.</t>
+          <t>Бердичівський нотаріус М. Д. Клинковштейн м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C429" s="27" t="inlineStr">
@@ -12830,7 +12830,7 @@
       </c>
       <c r="B430" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv notary NE Martos, Berdychiv, Kiev Lips.</t>
+          <t>Бердичівський нотаріус Н. Є. Мартос м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C430" s="27" t="inlineStr">
@@ -12857,7 +12857,7 @@
       </c>
       <c r="B431" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv notary VG Gritsayev, Berdychiv, Kiev Lips.</t>
+          <t>Бердичівський нотаріус В. Г. Грицаєв м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C431" s="27" t="inlineStr">
@@ -12884,7 +12884,7 @@
       </c>
       <c r="B432" s="6" t="inlineStr">
         <is>
-          <t>Korninsky Sugar Factory Kornin, Skvyrsky floor.</t>
+          <t>Корнинський цукровий завод с. Корнин, Сквирського пов.</t>
         </is>
       </c>
       <c r="C432" s="27" t="inlineStr">
@@ -12911,7 +12911,7 @@
       </c>
       <c r="B433" s="6" t="inlineStr">
         <is>
-          <t>Judicial Investigator of Berdichev, Kiev Lips.</t>
+          <t>Судовий слідчий м. Бердичева, Київської губ.</t>
         </is>
       </c>
       <c r="C433" s="27" t="inlineStr">
@@ -12938,7 +12938,7 @@
       </c>
       <c r="B434" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv notary II Ploskonny, Berdychiv, Kiev Lips.</t>
+          <t>Бердичівський нотаріус І. І. Плосконний м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C434" s="27" t="inlineStr">
@@ -12965,7 +12965,7 @@
       </c>
       <c r="B435" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv notary AF Plat a Berdychiv, Kiev Lips.</t>
+          <t>Бердичівський нотаріус А. Ф. Платер м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C435" s="27" t="inlineStr">
@@ -12992,7 +12992,7 @@
       </c>
       <c r="B436" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv notary VV Kaminsky, Berdychiv, Kiev Lips.</t>
+          <t>Бердичівський нотаріус В. В. Камінський м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C436" s="27" t="inlineStr">
@@ -13019,7 +13019,7 @@
       </c>
       <c r="B437" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv notary AA Vilensky, Berdychiv, Kiev Lips.</t>
+          <t>Бердичівський нотаріус А. А. Віленський м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C437" s="27" t="inlineStr">
@@ -13046,7 +13046,7 @@
       </c>
       <c r="B438" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv notary VI Ignatiev city of Berdychiv, Kiev lips.</t>
+          <t>Бердичівський нотаріус В. І. Ігнатьєв м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C438" s="27" t="inlineStr">
@@ -13073,7 +13073,7 @@
       </c>
       <c r="B439" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv notary TA Pogrebetsky in Berdychiv, Kiev lips.</t>
+          <t>Бердичівський нотаріус Т. А. Погребецький м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C439" s="27" t="inlineStr">
@@ -13100,7 +13100,7 @@
       </c>
       <c r="B440" s="6" t="inlineStr">
         <is>
-          <t>Berdychiv notary DV NEBOLSIN in Berdychiv, Kyiv Lips.</t>
+          <t>Бердичівський нотаріус Д. В. Нєбольсин м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C440" s="27" t="inlineStr">
@@ -13127,7 +13127,7 @@
       </c>
       <c r="B441" s="6" t="inlineStr">
         <is>
-          <t>Church of the Nativity of the Virgin Mary of Andrushevka, Zhytomyr</t>
+          <t>Церква Різдва Богородиці м-ка Андрушівка, Житомирського пов.</t>
         </is>
       </c>
       <c r="C441" s="27" t="inlineStr">
@@ -13154,7 +13154,7 @@
       </c>
       <c r="B442" s="6" t="inlineStr">
         <is>
-          <t>St. Nikolaev Church of Berdychiv, Kiev Lips.</t>
+          <t>Св. Миколаївська церква м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C442" s="27" t="inlineStr">
@@ -13181,7 +13181,7 @@
       </c>
       <c r="B443" s="6" t="inlineStr">
         <is>
-          <t>Miropolsky County Court of Miropolier, Kursk Lips.</t>
+          <t>Миропольський повітовий суд м. Миропольє, Курської губ.</t>
         </is>
       </c>
       <c r="C443" s="27" t="inlineStr">
@@ -13208,7 +13208,7 @@
       </c>
       <c r="B444" s="6" t="inlineStr">
         <is>
-          <t>Fitinsky Orest Avksentievich, teacher of Zhytomyr Women's Theological School</t>
+          <t>Фотинський Орест Авксентійович, викладач Житомирського жіночого духовного училища</t>
         </is>
       </c>
       <c r="C444" s="27" t="inlineStr">
@@ -13235,7 +13235,7 @@
       </c>
       <c r="B445" s="6" t="inlineStr">
         <is>
-          <t>Radomysl Highway Magistrate, Radomysl, Kiev Lips.</t>
+          <t>Радомисльський городовий магістрат м. Радомисль, Київської губ.</t>
         </is>
       </c>
       <c r="C445" s="27" t="inlineStr">
@@ -13262,7 +13262,7 @@
       </c>
       <c r="B446" s="6" t="inlineStr">
         <is>
-          <t>Brovkovsky District Board of the village. Brovka, Skvyrsky floor.</t>
+          <t>Бровківське волосне правління с. Бровки, Сквирського пов.</t>
         </is>
       </c>
       <c r="C446" s="27" t="inlineStr">
@@ -13289,7 +13289,7 @@
       </c>
       <c r="B447" s="6" t="inlineStr">
         <is>
-          <t>Radomysl County for Elections to the 2nd State Duma Commission of Radomysl, Kyiv Lips</t>
+          <t>Радомисльська повітова у справах про вибори до 2-ої Державної Думи комісія м. Радомисль, Київської губ</t>
         </is>
       </c>
       <c r="C447" s="27" t="inlineStr">
@@ -13316,7 +13316,7 @@
       </c>
       <c r="B448" s="6" t="inlineStr">
         <is>
-          <t>Radomysl City Police. Radomysl, Kiev Lips</t>
+          <t>Радомисльська міська поліція. Радомисль, Київської губ</t>
         </is>
       </c>
       <c r="C448" s="27" t="inlineStr">
@@ -13343,7 +13343,7 @@
       </c>
       <c r="B449" s="6" t="inlineStr">
         <is>
-          <t>The first Radomysl county in the chin cases is the city of Radomysl, the Kiev lips.</t>
+          <t>Перше Радомисльське повітове у чиншових справах присутствіє м. Радомисль, Київської губ.</t>
         </is>
       </c>
       <c r="C449" s="27" t="inlineStr">
@@ -13370,7 +13370,7 @@
       </c>
       <c r="B450" s="6" t="inlineStr">
         <is>
-          <t>Brusyliv District Board of Brusyliv, Radomysl Plo.</t>
+          <t>Брусилівське волосне правління м-ко Брусилів, Радомисльського пов.</t>
         </is>
       </c>
       <c r="C450" s="27" t="inlineStr">
@@ -13397,7 +13397,7 @@
       </c>
       <c r="B451" s="6" t="inlineStr">
         <is>
-          <t>The Media Mediator of the 1st District of Radomysl County</t>
+          <t>Мировий посередник 1-ої дільниці Радомисльського повіту</t>
         </is>
       </c>
       <c r="C451" s="27" t="inlineStr">
@@ -13424,7 +13424,7 @@
       </c>
       <c r="B452" s="6" t="inlineStr">
         <is>
-          <t>The Medical Mediator of the 2nd District of Radomysl Plo.</t>
+          <t>Мировий посередник 2-ої дільниці Радомисльського пов.</t>
         </is>
       </c>
       <c r="C452" s="27" t="inlineStr">
@@ -13451,7 +13451,7 @@
       </c>
       <c r="B453" s="6" t="inlineStr">
         <is>
-          <t>The Radomysl County Recart is present in Radomysl, Kyiv Lips.</t>
+          <t>Радомисльське повітове рекртське присутствіє м. Радомисль, Київської губ.</t>
         </is>
       </c>
       <c r="C453" s="27" t="inlineStr">
@@ -13478,7 +13478,7 @@
       </c>
       <c r="B454" s="6" t="inlineStr">
         <is>
-          <t>Korninskaya bourgeois administration p. Kornin, Skvyrsky floor.</t>
+          <t>Корнинська міщанська управа с. Корнин, Сквирського пов.</t>
         </is>
       </c>
       <c r="C454" s="27" t="inlineStr">
@@ -13505,7 +13505,7 @@
       </c>
       <c r="B455" s="6" t="inlineStr">
         <is>
-          <t>Radomysl County Soviet, Radomysl, Kiev Lips.</t>
+          <t>Радомисльський повітовий стряпчий м. Радомисль, Київської губ.</t>
         </is>
       </c>
       <c r="C455" s="27" t="inlineStr">
@@ -13532,7 +13532,7 @@
       </c>
       <c r="B456" s="6" t="inlineStr">
         <is>
-          <t>Radomysl district in cases of elections to the 4th State Duma Commission of Radomysl, Kiev Lips.</t>
+          <t>Радомисльська повітова у справах про вибори до 4-ої Державної Думи комісія м. Радомисль, Київської губ.</t>
         </is>
       </c>
       <c r="C456" s="27" t="inlineStr">
@@ -13559,7 +13559,7 @@
       </c>
       <c r="B457" s="6" t="inlineStr">
         <is>
-          <t>Kamyansky District Board of the village. Kamyanka, Radomysl district.</t>
+          <t>Кам'янське волосне правління с. Кам'янка, Радомисльського пов.</t>
         </is>
       </c>
       <c r="C457" s="27" t="inlineStr">
@@ -13586,7 +13586,7 @@
       </c>
       <c r="B458" s="6" t="inlineStr">
         <is>
-          <t>Radomysl district in cases of elections to the 1st State Duma Commission of Radomysl, Kyiv Lips.</t>
+          <t>Радомисльська повітова у справах про вибори до 1-ої Державної Думи комісія м. Радомисль, Київської губ.</t>
         </is>
       </c>
       <c r="C458" s="27" t="inlineStr">
@@ -13613,7 +13613,7 @@
       </c>
       <c r="B459" s="6" t="inlineStr">
         <is>
-          <t>Radomysl district in cases of elections to the 3rd State Duma Commission of Radomysl, Kyiv Lips.</t>
+          <t>Радомисльська повітова у справах про вибори до 3-ої Державної Думи комісія м. Радомисль, Київської губ.</t>
         </is>
       </c>
       <c r="C459" s="27" t="inlineStr">
@@ -13640,7 +13640,7 @@
       </c>
       <c r="B460" s="6" t="inlineStr">
         <is>
-          <t>The Boarding Board of the Mischansky Board of the M-Ku, Skvyrskaya St.</t>
+          <t>Вчорайшенська міщанська управа м-ко Вчорайше, Сквирського пов.</t>
         </is>
       </c>
       <c r="C460" s="27" t="inlineStr">
@@ -13667,7 +13667,7 @@
       </c>
       <c r="B461" s="6" t="inlineStr">
         <is>
-          <t>The 2nd state of the Radomysl district, the Kiev lips.</t>
+          <t>Пристав 2-го стану Радомисльського пов.,  Київської губ.</t>
         </is>
       </c>
       <c r="C461" s="27" t="inlineStr">
@@ -13694,7 +13694,7 @@
       </c>
       <c r="B462" s="6" t="inlineStr">
         <is>
-          <t>Comrade of the Prosecutor of the Kyiv District Court at the Radomysl district of Radomysl, Kyiv Lips.</t>
+          <t>Товариш прокурора Київського окружного суду по Радомисльській дільниці м. Радомисль, Київської губ.</t>
         </is>
       </c>
       <c r="C462" s="27" t="inlineStr">
@@ -13721,7 +13721,7 @@
       </c>
       <c r="B463" s="6" t="inlineStr">
         <is>
-          <t>Competitive Court of Radomysl County of Radomysl, Kiev Lips.</t>
+          <t>Конкурсний суд Радомисльського повіту м. Радомисль, Київської губ.</t>
         </is>
       </c>
       <c r="C463" s="27" t="inlineStr">
@@ -13748,7 +13748,7 @@
       </c>
       <c r="B464" s="6" t="inlineStr">
         <is>
-          <t>Radomysl notary AK Melenevsky, Radomysl, Kiev Lips.</t>
+          <t>Радомисльський нотаріус А. К. Меленевський м. Радомисль, Київської губ.</t>
         </is>
       </c>
       <c r="C464" s="27" t="inlineStr">
@@ -13775,7 +13775,7 @@
       </c>
       <c r="B465" s="6" t="inlineStr">
         <is>
-          <t>Radomysl notary KF Grigoryev, Radomysl, Kiev Lips.</t>
+          <t>Радомисльський нотаріус К. Ф. Григорьєв м. Радомисль, Київської губ.</t>
         </is>
       </c>
       <c r="C465" s="27" t="inlineStr">
@@ -13802,7 +13802,7 @@
       </c>
       <c r="B466" s="6" t="inlineStr">
         <is>
-          <t>Khodorkovsky notary AF Ivanov M-ko Khodorkiv, Skvyrsky district.</t>
+          <t>Ходорківський нотаріус А. Ф. Іванов м-ко Ходорків, Сквирського пов.</t>
         </is>
       </c>
       <c r="C466" s="27" t="inlineStr">
@@ -13829,7 +13829,7 @@
       </c>
       <c r="B467" s="6" t="inlineStr">
         <is>
-          <t>Radomysl County Agemir of Radomysl, Kiev Lips.</t>
+          <t>Радомисльський повітовий землемір м. Радомисль, Київської губ.</t>
         </is>
       </c>
       <c r="C467" s="27" t="inlineStr">
@@ -13856,7 +13856,7 @@
       </c>
       <c r="B468" s="6" t="inlineStr">
         <is>
-          <t>Society of Yanushpilsky Sugar Broad Plant of Yanushpil, Zhytomyr district.</t>
+          <t>Товариство Янушпільського цукробурякового заводу м-ко Янушпіль, Житомирського пов.</t>
         </is>
       </c>
       <c r="C468" s="27" t="inlineStr">
@@ -13883,7 +13883,7 @@
       </c>
       <c r="B469" s="6" t="inlineStr">
         <is>
-          <t>Radomysl County Food Administration of Radomysl, Kiev Lips.</t>
+          <t>Радомисльська повітова продовольча управа м. Радомисль, Київської губ.</t>
         </is>
       </c>
       <c r="C469" s="27" t="inlineStr">
@@ -13910,7 +13910,7 @@
       </c>
       <c r="B470" s="6" t="inlineStr">
         <is>
-          <t>Malinskaya District Food Administration M-KO Malin, Radomysl district.</t>
+          <t>Малинська волосна продовольча управа м-ко Малин, Радомисльського пов.</t>
         </is>
       </c>
       <c r="C470" s="27" t="inlineStr">
@@ -13937,7 +13937,7 @@
       </c>
       <c r="B471" s="6" t="inlineStr">
         <is>
-          <t>Radomysl County Peace Congress of Radomysl, Kiev Lips.</t>
+          <t>Радомисльський повітовий мировий з'їзд м. Радомисль, Київської губ.</t>
         </is>
       </c>
       <c r="C471" s="27" t="inlineStr">
@@ -13964,7 +13964,7 @@
       </c>
       <c r="B472" s="6" t="inlineStr">
         <is>
-          <t>Comrade of the Prakuror of the Kiev District Court at the Berdychiv district of Berdychiv, Kiev lips.</t>
+          <t>Товариш пркурора Київського окружного суду по Бердичівській дільниці м. Бердичів, Київської губ.</t>
         </is>
       </c>
       <c r="C472" s="27" t="inlineStr">
@@ -13991,7 +13991,7 @@
       </c>
       <c r="B473" s="6" t="inlineStr">
         <is>
-          <t>Rusanovsky village administration of the village. Rusanivka, Radomysl district.</t>
+          <t>Русанівське сільське управління с. Русанівка, Радомисльського пов.</t>
         </is>
       </c>
       <c r="C473" s="27" t="inlineStr">
@@ -14018,7 +14018,7 @@
       </c>
       <c r="B474" s="6" t="inlineStr">
         <is>
-          <t>Kropyvnya village administration of the village. Kropyvnya, Radomysl district, Kiev lips.</t>
+          <t>Кропивнянське сільське управління с. Кропивня, Радомисльського пов., Київської губ.</t>
         </is>
       </c>
       <c r="C474" s="27" t="inlineStr">
@@ -14045,7 +14045,7 @@
       </c>
       <c r="B475" s="6" t="inlineStr">
         <is>
-          <t>Ruzhyn bourgeois administration M-ko Ruzhin. Berdichevsky str.</t>
+          <t>Ружинська міщанська управа м-ко Ружин. Бердичівського пов.</t>
         </is>
       </c>
       <c r="C475" s="27" t="inlineStr">
@@ -14072,7 +14072,7 @@
       </c>
       <c r="B476" s="6" t="inlineStr">
         <is>
-          <t>Gorbul District Board of the village. Gorbula, Radomysl district.</t>
+          <t>Горбулівське волосне правління с. Горбулів, Радомисльського пов.</t>
         </is>
       </c>
       <c r="C476" s="27" t="inlineStr">
@@ -14099,7 +14099,7 @@
       </c>
       <c r="B477" s="6" t="inlineStr">
         <is>
-          <t>Irshansk Postal and Telegraph Office of the Kiev Postal and Telegraph District</t>
+          <t>Іршанське поштово-телеграфне відділення Київського поштово-телеграфного округу</t>
         </is>
       </c>
       <c r="C477" s="27" t="inlineStr">
@@ -14126,7 +14126,7 @@
       </c>
       <c r="B478" s="6" t="inlineStr">
         <is>
-          <t>Stremygorod postal and telegraph office of the Kiev Postal and Telegraph District. Stremigorod, Radomysl district.</t>
+          <t>Стремигородська поштово-телеграфна контора Київського поштово-телеграфного округу с. Стремигород, Радомисльського пов.</t>
         </is>
       </c>
       <c r="C478" s="27" t="inlineStr">
@@ -14153,7 +14153,7 @@
       </c>
       <c r="B479" s="6" t="inlineStr">
         <is>
-          <t>The Bolotsk Board Administration M-Ka Pavoloch, Skvyrsky district.</t>
+          <t>Паволоцька міщанська управа м-ко Паволоч, Сквирського пов.</t>
         </is>
       </c>
       <c r="C479" s="27" t="inlineStr">
@@ -14180,7 +14180,7 @@
       </c>
       <c r="B480" s="6" t="inlineStr">
         <is>
-          <t>Collection of Talmud-Ttor Zhytomyr, Zhytomyr Region</t>
+          <t>Колекція Талмуд-Тор м. Житомир, Житомирської обл.</t>
         </is>
       </c>
       <c r="C480" s="27" t="inlineStr"/>
@@ -14203,7 +14203,7 @@
       </c>
       <c r="B481" s="6" t="inlineStr">
         <is>
-          <t>Collection of cartographic materials of Zhytomyr, Zhytomyr region</t>
+          <t>Колекція картографічних матеріалів м. Житомир, Житомирської обл.</t>
         </is>
       </c>
       <c r="C481" s="27" t="inlineStr">

</xml_diff>